<commit_message>
add more to numtx treatment, reduce dropout and increase care linkage
</commit_message>
<xml_diff>
--- a/tests/cascade2p.xlsx
+++ b/tests/cascade2p.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="11"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" state="visible" r:id="rId2"/>
@@ -149,7 +149,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="118">
   <si>
     <t>O P T I M A</t>
   </si>
@@ -271,16 +271,28 @@
     <t>Percentage of people in care who are lost to follow-up per year (%/year)</t>
   </si>
   <si>
+    <t>Viral suppression – ART initiators (%)</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Biological failure rate (%/year)</t>
+  </si>
+  <si>
+    <t>Viral load monitoring (number/year)</t>
+  </si>
+  <si>
+    <t>Time to ART re-initiation (years)</t>
+  </si>
+  <si>
+    <t>PLHIV aware of their status (%)</t>
+  </si>
+  <si>
     <t>Percentage of HIV-diagnosed people who are in care (%)</t>
   </si>
   <si>
-    <t>Average</t>
-  </si>
-  <si>
     <t>Proportion of people on ART with viral suppression (%)</t>
-  </si>
-  <si>
-    <t>Biological failure rate (%/year)</t>
   </si>
   <si>
     <t>Percentage of population tested for HIV in the last 12 months</t>
@@ -497,13 +509,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
+  <numFmts count="7">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="0"/>
     <numFmt numFmtId="166" formatCode="0.00E+00"/>
     <numFmt numFmtId="167" formatCode="0.00%"/>
     <numFmt numFmtId="168" formatCode="#,##0.00"/>
     <numFmt numFmtId="169" formatCode="0%"/>
+    <numFmt numFmtId="170" formatCode="#,##0.0"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -656,7 +669,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -730,6 +743,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="169" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -850,15 +867,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>108000</xdr:colOff>
+      <xdr:colOff>351000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>182880</xdr:colOff>
+      <xdr:colOff>422640</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>36720</xdr:rowOff>
+      <xdr:rowOff>33480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -867,8 +884,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="108000" y="0"/>
-          <a:ext cx="13282560" cy="7123320"/>
+          <a:off x="351000" y="0"/>
+          <a:ext cx="25572960" cy="7120080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -895,15 +912,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>108000</xdr:colOff>
+      <xdr:colOff>351000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>182880</xdr:colOff>
+      <xdr:colOff>422640</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>36720</xdr:rowOff>
+      <xdr:rowOff>33480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -912,8 +929,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="108000" y="0"/>
-          <a:ext cx="13282560" cy="7123320"/>
+          <a:off x="351000" y="0"/>
+          <a:ext cx="25572960" cy="7120080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -940,15 +957,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>108000</xdr:colOff>
+      <xdr:colOff>351000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>182880</xdr:colOff>
+      <xdr:colOff>422640</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>36720</xdr:rowOff>
+      <xdr:rowOff>33480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -957,8 +974,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="108000" y="0"/>
-          <a:ext cx="13282560" cy="7123320"/>
+          <a:off x="351000" y="0"/>
+          <a:ext cx="25572960" cy="7120080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -985,15 +1002,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>108000</xdr:colOff>
+      <xdr:colOff>351000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>182880</xdr:colOff>
+      <xdr:colOff>422640</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>36720</xdr:rowOff>
+      <xdr:rowOff>33480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1002,8 +1019,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="108000" y="0"/>
-          <a:ext cx="13282560" cy="7123320"/>
+          <a:off x="351000" y="0"/>
+          <a:ext cx="25572960" cy="7120080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1030,15 +1047,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>108000</xdr:colOff>
+      <xdr:colOff>351000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>182880</xdr:colOff>
+      <xdr:colOff>422640</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>36720</xdr:rowOff>
+      <xdr:rowOff>33480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1047,8 +1064,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="108000" y="0"/>
-          <a:ext cx="13282560" cy="7123320"/>
+          <a:off x="351000" y="0"/>
+          <a:ext cx="25572960" cy="7120080"/>
         </a:xfrm>
         <a:solidFill>
           <a:srgbClr val="ffffff"/>
@@ -1077,15 +1094,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>108000</xdr:colOff>
+      <xdr:colOff>351000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>182880</xdr:colOff>
+      <xdr:colOff>422640</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>36720</xdr:rowOff>
+      <xdr:rowOff>33480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1094,8 +1111,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="108000" y="0"/>
-          <a:ext cx="13282560" cy="7313760"/>
+          <a:off x="351000" y="0"/>
+          <a:ext cx="25572960" cy="7310520"/>
         </a:xfrm>
         <a:solidFill>
           <a:srgbClr val="ffffff"/>
@@ -1124,15 +1141,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>108000</xdr:colOff>
+      <xdr:colOff>351000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>182880</xdr:colOff>
+      <xdr:colOff>422640</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>93960</xdr:rowOff>
+      <xdr:rowOff>90720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1141,8 +1158,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="108000" y="0"/>
-          <a:ext cx="13282560" cy="8437680"/>
+          <a:off x="351000" y="0"/>
+          <a:ext cx="25572960" cy="8434440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1169,15 +1186,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>108000</xdr:colOff>
+      <xdr:colOff>351000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>182880</xdr:colOff>
+      <xdr:colOff>422640</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>93960</xdr:rowOff>
+      <xdr:rowOff>90720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1186,8 +1203,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="108000" y="0"/>
-          <a:ext cx="13282560" cy="8437680"/>
+          <a:off x="351000" y="0"/>
+          <a:ext cx="25572960" cy="8434440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1214,15 +1231,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>108000</xdr:colOff>
+      <xdr:colOff>351000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>182880</xdr:colOff>
+      <xdr:colOff>422640</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>93960</xdr:rowOff>
+      <xdr:rowOff>90720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1231,8 +1248,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="108000" y="0"/>
-          <a:ext cx="13282560" cy="8437680"/>
+          <a:off x="351000" y="0"/>
+          <a:ext cx="25572960" cy="8434440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1259,15 +1276,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>108000</xdr:colOff>
+      <xdr:colOff>351000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>182880</xdr:colOff>
+      <xdr:colOff>422640</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>93960</xdr:rowOff>
+      <xdr:rowOff>90720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1276,8 +1293,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="108000" y="0"/>
-          <a:ext cx="13282560" cy="8437680"/>
+          <a:off x="351000" y="0"/>
+          <a:ext cx="25572960" cy="8434440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1304,15 +1321,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>108000</xdr:colOff>
+      <xdr:colOff>351000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>182880</xdr:colOff>
+      <xdr:colOff>422640</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>93960</xdr:rowOff>
+      <xdr:rowOff>90720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1321,8 +1338,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="108000" y="0"/>
-          <a:ext cx="13282560" cy="9771120"/>
+          <a:off x="351000" y="0"/>
+          <a:ext cx="25572960" cy="9767880"/>
         </a:xfrm>
         <a:solidFill>
           <a:srgbClr val="ffffff"/>
@@ -1351,15 +1368,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>108000</xdr:colOff>
+      <xdr:colOff>351000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>182880</xdr:colOff>
+      <xdr:colOff>422640</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>55800</xdr:rowOff>
+      <xdr:rowOff>52560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1368,8 +1385,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="108000" y="0"/>
-          <a:ext cx="13282560" cy="7809120"/>
+          <a:off x="351000" y="0"/>
+          <a:ext cx="25572960" cy="7805880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1396,15 +1413,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>108000</xdr:colOff>
+      <xdr:colOff>351000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>182880</xdr:colOff>
+      <xdr:colOff>422640</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>55800</xdr:rowOff>
+      <xdr:rowOff>52560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1413,8 +1430,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="108000" y="0"/>
-          <a:ext cx="13282560" cy="7809120"/>
+          <a:off x="351000" y="0"/>
+          <a:ext cx="25572960" cy="7805880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1441,15 +1458,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>108000</xdr:colOff>
+      <xdr:colOff>351000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>182880</xdr:colOff>
+      <xdr:colOff>422640</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>55800</xdr:rowOff>
+      <xdr:rowOff>52560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1458,8 +1475,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="108000" y="0"/>
-          <a:ext cx="13282560" cy="7809120"/>
+          <a:off x="351000" y="0"/>
+          <a:ext cx="25572960" cy="7805880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1486,15 +1503,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>108000</xdr:colOff>
+      <xdr:colOff>351000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>182880</xdr:colOff>
+      <xdr:colOff>422640</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>55800</xdr:rowOff>
+      <xdr:rowOff>52560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1503,8 +1520,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="108000" y="0"/>
-          <a:ext cx="13282560" cy="7809120"/>
+          <a:off x="351000" y="0"/>
+          <a:ext cx="25572960" cy="7805880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1531,15 +1548,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>108000</xdr:colOff>
+      <xdr:colOff>351000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>182880</xdr:colOff>
+      <xdr:colOff>422640</xdr:colOff>
       <xdr:row>55</xdr:row>
-      <xdr:rowOff>55800</xdr:rowOff>
+      <xdr:rowOff>52560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1548,8 +1565,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="108000" y="0"/>
-          <a:ext cx="13282560" cy="10095120"/>
+          <a:off x="351000" y="0"/>
+          <a:ext cx="25572960" cy="10091880"/>
         </a:xfrm>
         <a:solidFill>
           <a:srgbClr val="ffffff"/>
@@ -1578,15 +1595,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>108000</xdr:colOff>
+      <xdr:colOff>351000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>182880</xdr:colOff>
+      <xdr:colOff>422640</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>93960</xdr:rowOff>
+      <xdr:rowOff>90720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1595,8 +1612,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="108000" y="0"/>
-          <a:ext cx="13282560" cy="9866520"/>
+          <a:off x="351000" y="0"/>
+          <a:ext cx="25572960" cy="9863280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1623,15 +1640,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>108000</xdr:colOff>
+      <xdr:colOff>351000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>182880</xdr:colOff>
+      <xdr:colOff>422640</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>93960</xdr:rowOff>
+      <xdr:rowOff>90720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1640,8 +1657,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="108000" y="0"/>
-          <a:ext cx="13282560" cy="9866520"/>
+          <a:off x="351000" y="0"/>
+          <a:ext cx="25572960" cy="9863280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1668,15 +1685,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>108000</xdr:colOff>
+      <xdr:colOff>351000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>182880</xdr:colOff>
+      <xdr:colOff>422640</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>93960</xdr:rowOff>
+      <xdr:rowOff>90720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1685,8 +1702,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="108000" y="0"/>
-          <a:ext cx="13282560" cy="9866520"/>
+          <a:off x="351000" y="0"/>
+          <a:ext cx="25572960" cy="9863280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1713,15 +1730,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>108000</xdr:colOff>
+      <xdr:colOff>351000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>182880</xdr:colOff>
+      <xdr:colOff>422640</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>93960</xdr:rowOff>
+      <xdr:rowOff>90720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1730,8 +1747,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="108000" y="0"/>
-          <a:ext cx="13282560" cy="9866520"/>
+          <a:off x="351000" y="0"/>
+          <a:ext cx="25572960" cy="9863280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1758,15 +1775,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>108000</xdr:colOff>
+      <xdr:colOff>351000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>182880</xdr:colOff>
+      <xdr:colOff>422640</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>93960</xdr:rowOff>
+      <xdr:rowOff>90720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1775,8 +1792,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="108000" y="0"/>
-          <a:ext cx="13282560" cy="9866520"/>
+          <a:off x="351000" y="0"/>
+          <a:ext cx="25572960" cy="9863280"/>
         </a:xfrm>
         <a:solidFill>
           <a:srgbClr val="ffffff"/>
@@ -1813,8 +1830,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="121.908163265306"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.86224489795918"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="244.15306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="19.265306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1871,13 +1888,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="35" min="1" style="0" width="11.6989795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="36" style="0" width="9.86224489795918"/>
+    <col collapsed="false" hidden="false" max="35" min="1" style="0" width="22.5867346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="36" style="0" width="19.265306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2066,7 +2083,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2172,41 +2189,41 @@
         <f aca="false">Populations!$C$3</f>
         <v>M 15-49</v>
       </c>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="19"/>
-      <c r="M10" s="19"/>
-      <c r="N10" s="19"/>
-      <c r="O10" s="19"/>
-      <c r="P10" s="19"/>
-      <c r="Q10" s="19"/>
-      <c r="R10" s="19"/>
-      <c r="S10" s="19"/>
-      <c r="T10" s="19"/>
-      <c r="U10" s="19"/>
-      <c r="V10" s="19"/>
-      <c r="W10" s="19"/>
-      <c r="X10" s="19"/>
-      <c r="Y10" s="19"/>
-      <c r="Z10" s="19"/>
-      <c r="AA10" s="19"/>
-      <c r="AB10" s="19"/>
-      <c r="AC10" s="19"/>
-      <c r="AD10" s="19"/>
-      <c r="AE10" s="19"/>
-      <c r="AF10" s="19"/>
-      <c r="AG10" s="19"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="20"/>
+      <c r="O10" s="20"/>
+      <c r="P10" s="20"/>
+      <c r="Q10" s="20"/>
+      <c r="R10" s="20"/>
+      <c r="S10" s="20"/>
+      <c r="T10" s="20"/>
+      <c r="U10" s="20"/>
+      <c r="V10" s="20"/>
+      <c r="W10" s="20"/>
+      <c r="X10" s="20"/>
+      <c r="Y10" s="20"/>
+      <c r="Z10" s="20"/>
+      <c r="AA10" s="20"/>
+      <c r="AB10" s="20"/>
+      <c r="AC10" s="20"/>
+      <c r="AD10" s="20"/>
+      <c r="AE10" s="20"/>
+      <c r="AF10" s="20"/>
+      <c r="AG10" s="20"/>
       <c r="AH10" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="AI10" s="19" t="n">
+      <c r="AI10" s="20" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2215,47 +2232,47 @@
         <f aca="false">Populations!$C$4</f>
         <v>F 15-49</v>
       </c>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19"/>
-      <c r="L11" s="19"/>
-      <c r="M11" s="19"/>
-      <c r="N11" s="19"/>
-      <c r="O11" s="19"/>
-      <c r="P11" s="19"/>
-      <c r="Q11" s="19"/>
-      <c r="R11" s="19"/>
-      <c r="S11" s="19"/>
-      <c r="T11" s="19"/>
-      <c r="U11" s="19"/>
-      <c r="V11" s="19"/>
-      <c r="W11" s="19"/>
-      <c r="X11" s="19"/>
-      <c r="Y11" s="19"/>
-      <c r="Z11" s="19"/>
-      <c r="AA11" s="19"/>
-      <c r="AB11" s="19"/>
-      <c r="AC11" s="19"/>
-      <c r="AD11" s="19"/>
-      <c r="AE11" s="19"/>
-      <c r="AF11" s="19"/>
-      <c r="AG11" s="19"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="20"/>
+      <c r="O11" s="20"/>
+      <c r="P11" s="20"/>
+      <c r="Q11" s="20"/>
+      <c r="R11" s="20"/>
+      <c r="S11" s="20"/>
+      <c r="T11" s="20"/>
+      <c r="U11" s="20"/>
+      <c r="V11" s="20"/>
+      <c r="W11" s="20"/>
+      <c r="X11" s="20"/>
+      <c r="Y11" s="20"/>
+      <c r="Z11" s="20"/>
+      <c r="AA11" s="20"/>
+      <c r="AB11" s="20"/>
+      <c r="AC11" s="20"/>
+      <c r="AD11" s="20"/>
+      <c r="AE11" s="20"/>
+      <c r="AF11" s="20"/>
+      <c r="AG11" s="20"/>
       <c r="AH11" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="AI11" s="19" t="n">
+      <c r="AI11" s="20" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2422,15 +2439,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.6989795918367"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="16.9744897959184"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="11.6989795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.86224489795918"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="22.5867346938776"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="33.6020408163265"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="22.5867346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="19.265306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
@@ -2477,7 +2494,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -2524,7 +2541,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -2569,7 +2586,7 @@
     </row>
     <row r="22" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
@@ -2602,7 +2619,7 @@
     </row>
     <row r="29" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -2659,20 +2676,20 @@
   </sheetPr>
   <dimension ref="A1:I79"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A36" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A36" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B45" activeCellId="0" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.86224489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.1683673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.86224489795918"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.265306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="110.780612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="19.265306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="15" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2687,100 +2704,100 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B3" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="C3" s="26" t="n">
+      <c r="B3" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="27" t="n">
         <v>0.0004</v>
       </c>
-      <c r="D3" s="26" t="n">
+      <c r="D3" s="27" t="n">
         <v>0.0001</v>
       </c>
-      <c r="E3" s="26" t="n">
+      <c r="E3" s="27" t="n">
         <v>0.0014</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="C4" s="26" t="n">
+      <c r="B4" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="27" t="n">
         <v>0.0008</v>
       </c>
-      <c r="D4" s="26" t="n">
+      <c r="D4" s="27" t="n">
         <v>0.0006</v>
       </c>
-      <c r="E4" s="26" t="n">
+      <c r="E4" s="27" t="n">
         <v>0.0011</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="C5" s="26" t="n">
+      <c r="B5" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" s="27" t="n">
         <v>0.0138</v>
       </c>
-      <c r="D5" s="26" t="n">
+      <c r="D5" s="27" t="n">
         <v>0.0102</v>
       </c>
-      <c r="E5" s="26" t="n">
+      <c r="E5" s="27" t="n">
         <v>0.0186</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="C6" s="26" t="n">
+      <c r="B6" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="27" t="n">
         <v>0.0011</v>
       </c>
-      <c r="D6" s="26" t="n">
+      <c r="D6" s="27" t="n">
         <v>0.0004</v>
       </c>
-      <c r="E6" s="26" t="n">
+      <c r="E6" s="27" t="n">
         <v>0.0028</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="C7" s="26" t="n">
+      <c r="B7" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" s="27" t="n">
         <v>0.008</v>
       </c>
-      <c r="D7" s="26" t="n">
+      <c r="D7" s="27" t="n">
         <v>0.0063</v>
       </c>
-      <c r="E7" s="26" t="n">
+      <c r="E7" s="27" t="n">
         <v>0.024</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="C8" s="26" t="n">
+      <c r="B8" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" s="27" t="n">
         <v>0.367</v>
       </c>
-      <c r="D8" s="26" t="n">
+      <c r="D8" s="27" t="n">
         <v>0.294</v>
       </c>
-      <c r="E8" s="26" t="n">
+      <c r="E8" s="27" t="n">
         <v>0.44</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="C9" s="26" t="n">
+      <c r="B9" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" s="27" t="n">
         <v>0.205</v>
       </c>
-      <c r="D9" s="26" t="n">
+      <c r="D9" s="27" t="n">
         <v>0.14</v>
       </c>
-      <c r="E9" s="26" t="n">
+      <c r="E9" s="27" t="n">
         <v>0.27</v>
       </c>
     </row>
@@ -2795,7 +2812,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="15" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2810,86 +2827,86 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="C15" s="27" t="n">
+      <c r="B15" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="C15" s="28" t="n">
         <v>26.03</v>
       </c>
-      <c r="D15" s="27" t="n">
+      <c r="D15" s="28" t="n">
         <v>2</v>
       </c>
-      <c r="E15" s="27" t="n">
+      <c r="E15" s="28" t="n">
         <v>48.02</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B16" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="C16" s="27" t="n">
+      <c r="B16" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" s="28" t="n">
         <v>1</v>
       </c>
-      <c r="D16" s="27" t="n">
+      <c r="D16" s="28" t="n">
         <v>1</v>
       </c>
-      <c r="E16" s="27" t="n">
+      <c r="E16" s="28" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B17" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="C17" s="27" t="n">
+      <c r="B17" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="C17" s="28" t="n">
         <v>1</v>
       </c>
-      <c r="D17" s="27" t="n">
+      <c r="D17" s="28" t="n">
         <v>1</v>
       </c>
-      <c r="E17" s="27" t="n">
+      <c r="E17" s="28" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B18" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="C18" s="27" t="n">
+      <c r="B18" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18" s="28" t="n">
         <v>1</v>
       </c>
-      <c r="D18" s="27" t="n">
+      <c r="D18" s="28" t="n">
         <v>1</v>
       </c>
-      <c r="E18" s="27" t="n">
+      <c r="E18" s="28" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B19" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="C19" s="27" t="n">
+      <c r="B19" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="C19" s="28" t="n">
         <v>3.49</v>
       </c>
-      <c r="D19" s="27" t="n">
+      <c r="D19" s="28" t="n">
         <v>1.76</v>
       </c>
-      <c r="E19" s="27" t="n">
+      <c r="E19" s="28" t="n">
         <v>6.92</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B20" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="C20" s="27" t="n">
+      <c r="B20" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20" s="28" t="n">
         <v>7.17</v>
       </c>
-      <c r="D20" s="27" t="n">
+      <c r="D20" s="28" t="n">
         <v>3.9</v>
       </c>
-      <c r="E20" s="27" t="n">
+      <c r="E20" s="28" t="n">
         <v>12.08</v>
       </c>
     </row>
@@ -2904,7 +2921,7 @@
     </row>
     <row r="24" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="15" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2919,8 +2936,8 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B26" s="25" t="s">
-        <v>82</v>
+      <c r="B26" s="26" t="s">
+        <v>86</v>
       </c>
       <c r="C26" s="18" t="n">
         <v>4.14</v>
@@ -2933,8 +2950,8 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B27" s="25" t="s">
-        <v>77</v>
+      <c r="B27" s="26" t="s">
+        <v>81</v>
       </c>
       <c r="C27" s="18" t="n">
         <v>1.05</v>
@@ -2947,8 +2964,8 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B28" s="25" t="s">
-        <v>83</v>
+      <c r="B28" s="26" t="s">
+        <v>87</v>
       </c>
       <c r="C28" s="18" t="n">
         <v>0.33</v>
@@ -2961,8 +2978,8 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B29" s="25" t="s">
-        <v>84</v>
+      <c r="B29" s="26" t="s">
+        <v>88</v>
       </c>
       <c r="C29" s="18" t="n">
         <v>0.27</v>
@@ -2975,8 +2992,8 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B30" s="25" t="s">
-        <v>85</v>
+      <c r="B30" s="26" t="s">
+        <v>89</v>
       </c>
       <c r="C30" s="18" t="n">
         <v>0.67</v>
@@ -2999,7 +3016,7 @@
     </row>
     <row r="34" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="15" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3014,8 +3031,8 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B36" s="25" t="s">
-        <v>87</v>
+      <c r="B36" s="26" t="s">
+        <v>91</v>
       </c>
       <c r="C36" s="18" t="n">
         <v>0.45</v>
@@ -3028,8 +3045,8 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B37" s="25" t="s">
-        <v>88</v>
+      <c r="B37" s="26" t="s">
+        <v>92</v>
       </c>
       <c r="C37" s="18" t="n">
         <v>0.7</v>
@@ -3042,8 +3059,8 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B38" s="25" t="s">
-        <v>89</v>
+      <c r="B38" s="26" t="s">
+        <v>93</v>
       </c>
       <c r="C38" s="18" t="n">
         <v>0.47</v>
@@ -3056,8 +3073,8 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B39" s="25" t="s">
-        <v>90</v>
+      <c r="B39" s="26" t="s">
+        <v>94</v>
       </c>
       <c r="C39" s="18" t="n">
         <v>1.52</v>
@@ -3080,7 +3097,7 @@
     </row>
     <row r="43" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="15" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3095,114 +3112,114 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B45" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="C45" s="26" t="n">
+      <c r="B45" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="C45" s="27" t="n">
         <v>0.0036</v>
       </c>
-      <c r="D45" s="26" t="n">
+      <c r="D45" s="27" t="n">
         <v>0.0029</v>
       </c>
-      <c r="E45" s="26" t="n">
+      <c r="E45" s="27" t="n">
         <v>0.0044</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B46" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="C46" s="26" t="n">
+      <c r="B46" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="C46" s="27" t="n">
         <v>0.0036</v>
       </c>
-      <c r="D46" s="26" t="n">
+      <c r="D46" s="27" t="n">
         <v>0.0029</v>
       </c>
-      <c r="E46" s="26" t="n">
+      <c r="E46" s="27" t="n">
         <v>0.0044</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B47" s="25" t="s">
-        <v>92</v>
-      </c>
-      <c r="C47" s="26" t="n">
+      <c r="B47" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="C47" s="27" t="n">
         <v>0.0058</v>
       </c>
-      <c r="D47" s="26" t="n">
+      <c r="D47" s="27" t="n">
         <v>0.0048</v>
       </c>
-      <c r="E47" s="26" t="n">
+      <c r="E47" s="27" t="n">
         <v>0.0071</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B48" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="C48" s="26" t="n">
+      <c r="B48" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="C48" s="27" t="n">
         <v>0.0088</v>
       </c>
-      <c r="D48" s="26" t="n">
+      <c r="D48" s="27" t="n">
         <v>0.075</v>
       </c>
-      <c r="E48" s="26" t="n">
+      <c r="E48" s="27" t="n">
         <v>0.0101</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B49" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="C49" s="26" t="n">
+      <c r="B49" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="C49" s="27" t="n">
         <v>0.059</v>
       </c>
-      <c r="D49" s="26" t="n">
+      <c r="D49" s="27" t="n">
         <v>0.054</v>
       </c>
-      <c r="E49" s="26" t="n">
+      <c r="E49" s="27" t="n">
         <v>0.079</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B50" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="C50" s="26" t="n">
+      <c r="B50" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="C50" s="27" t="n">
         <v>0.323</v>
       </c>
-      <c r="D50" s="26" t="n">
+      <c r="D50" s="27" t="n">
         <v>0.296</v>
       </c>
-      <c r="E50" s="26" t="n">
+      <c r="E50" s="27" t="n">
         <v>0.432</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B51" s="25" t="s">
-        <v>93</v>
-      </c>
-      <c r="C51" s="26" t="n">
+      <c r="B51" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="C51" s="27" t="n">
         <v>0.23</v>
       </c>
-      <c r="D51" s="26" t="n">
+      <c r="D51" s="27" t="n">
         <v>0.15</v>
       </c>
-      <c r="E51" s="26" t="n">
+      <c r="E51" s="27" t="n">
         <v>0.3</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B52" s="25" t="s">
-        <v>94</v>
-      </c>
-      <c r="C52" s="26" t="n">
+      <c r="B52" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="C52" s="27" t="n">
         <v>2.17</v>
       </c>
-      <c r="D52" s="26" t="n">
+      <c r="D52" s="27" t="n">
         <v>1.27</v>
       </c>
-      <c r="E52" s="26" t="n">
+      <c r="E52" s="27" t="n">
         <v>3.71</v>
       </c>
     </row>
@@ -3217,7 +3234,7 @@
     </row>
     <row r="56" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="15" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3232,8 +3249,8 @@
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B58" s="25" t="s">
-        <v>96</v>
+      <c r="B58" s="26" t="s">
+        <v>100</v>
       </c>
       <c r="C58" s="18" t="n">
         <v>0.95</v>
@@ -3244,13 +3261,13 @@
       <c r="E58" s="18" t="n">
         <v>0.98</v>
       </c>
-      <c r="G58" s="28"/>
-      <c r="H58" s="28"/>
-      <c r="I58" s="28"/>
+      <c r="G58" s="29"/>
+      <c r="H58" s="29"/>
+      <c r="I58" s="29"/>
     </row>
     <row r="59" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B59" s="25" t="s">
-        <v>97</v>
+      <c r="B59" s="26" t="s">
+        <v>101</v>
       </c>
       <c r="C59" s="18" t="n">
         <v>0.58</v>
@@ -3261,13 +3278,13 @@
       <c r="E59" s="18" t="n">
         <v>0.67</v>
       </c>
-      <c r="G59" s="28"/>
-      <c r="H59" s="28"/>
-      <c r="I59" s="28"/>
+      <c r="G59" s="29"/>
+      <c r="H59" s="29"/>
+      <c r="I59" s="29"/>
     </row>
     <row r="60" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B60" s="25" t="s">
-        <v>98</v>
+      <c r="B60" s="26" t="s">
+        <v>102</v>
       </c>
       <c r="C60" s="18" t="n">
         <v>0</v>
@@ -3278,13 +3295,13 @@
       <c r="E60" s="18" t="n">
         <v>0.68</v>
       </c>
-      <c r="G60" s="28"/>
-      <c r="H60" s="28"/>
-      <c r="I60" s="28"/>
+      <c r="G60" s="29"/>
+      <c r="H60" s="29"/>
+      <c r="I60" s="29"/>
     </row>
     <row r="61" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B61" s="25" t="s">
-        <v>99</v>
+      <c r="B61" s="26" t="s">
+        <v>103</v>
       </c>
       <c r="C61" s="18" t="n">
         <v>2.65</v>
@@ -3295,13 +3312,13 @@
       <c r="E61" s="18" t="n">
         <v>5.19</v>
       </c>
-      <c r="G61" s="28"/>
-      <c r="H61" s="28"/>
-      <c r="I61" s="28"/>
+      <c r="G61" s="29"/>
+      <c r="H61" s="29"/>
+      <c r="I61" s="29"/>
     </row>
     <row r="62" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B62" s="25" t="s">
-        <v>100</v>
+      <c r="B62" s="26" t="s">
+        <v>104</v>
       </c>
       <c r="C62" s="18" t="n">
         <v>0.54</v>
@@ -3312,13 +3329,13 @@
       <c r="E62" s="18" t="n">
         <v>0.68</v>
       </c>
-      <c r="G62" s="28"/>
-      <c r="H62" s="28"/>
-      <c r="I62" s="28"/>
+      <c r="G62" s="29"/>
+      <c r="H62" s="29"/>
+      <c r="I62" s="29"/>
     </row>
     <row r="63" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B63" s="25" t="s">
-        <v>101</v>
+      <c r="B63" s="26" t="s">
+        <v>105</v>
       </c>
       <c r="C63" s="18" t="n">
         <v>0.9</v>
@@ -3329,13 +3346,13 @@
       <c r="E63" s="18" t="n">
         <v>0.93</v>
       </c>
-      <c r="G63" s="28"/>
-      <c r="H63" s="28"/>
-      <c r="I63" s="28"/>
+      <c r="G63" s="29"/>
+      <c r="H63" s="29"/>
+      <c r="I63" s="29"/>
     </row>
     <row r="64" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B64" s="25" t="s">
-        <v>102</v>
+      <c r="B64" s="26" t="s">
+        <v>106</v>
       </c>
       <c r="C64" s="18" t="n">
         <v>0.73</v>
@@ -3346,13 +3363,13 @@
       <c r="E64" s="18" t="n">
         <v>0.8</v>
       </c>
-      <c r="G64" s="28"/>
-      <c r="H64" s="28"/>
-      <c r="I64" s="28"/>
+      <c r="G64" s="29"/>
+      <c r="H64" s="29"/>
+      <c r="I64" s="29"/>
     </row>
     <row r="65" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B65" s="25" t="s">
-        <v>103</v>
+      <c r="B65" s="26" t="s">
+        <v>107</v>
       </c>
       <c r="C65" s="18" t="n">
         <v>0.5</v>
@@ -3363,13 +3380,13 @@
       <c r="E65" s="18" t="n">
         <v>0.8</v>
       </c>
-      <c r="G65" s="28"/>
-      <c r="H65" s="28"/>
-      <c r="I65" s="28"/>
+      <c r="G65" s="29"/>
+      <c r="H65" s="29"/>
+      <c r="I65" s="29"/>
     </row>
     <row r="66" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B66" s="25" t="s">
-        <v>104</v>
+      <c r="B66" s="26" t="s">
+        <v>108</v>
       </c>
       <c r="C66" s="18" t="n">
         <v>0.92</v>
@@ -3382,8 +3399,8 @@
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B67" s="25" t="s">
-        <v>105</v>
+      <c r="B67" s="26" t="s">
+        <v>109</v>
       </c>
       <c r="C67" s="18" t="n">
         <v>0.9</v>
@@ -3400,7 +3417,7 @@
     </row>
     <row r="71" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="15" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3415,100 +3432,100 @@
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B73" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="C73" s="27" t="n">
+      <c r="B73" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="C73" s="28" t="n">
         <v>0.146</v>
       </c>
-      <c r="D73" s="27" t="n">
+      <c r="D73" s="28" t="n">
         <v>0.096</v>
       </c>
-      <c r="E73" s="27" t="n">
+      <c r="E73" s="28" t="n">
         <v>0.205</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B74" s="25" t="s">
-        <v>108</v>
-      </c>
-      <c r="C74" s="27" t="n">
+      <c r="B74" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="C74" s="28" t="n">
         <v>0.008</v>
       </c>
-      <c r="D74" s="27" t="n">
+      <c r="D74" s="28" t="n">
         <v>0.005</v>
       </c>
-      <c r="E74" s="27" t="n">
+      <c r="E74" s="28" t="n">
         <v>0.011</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B75" s="25" t="s">
-        <v>109</v>
-      </c>
-      <c r="C75" s="27" t="n">
+      <c r="B75" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="C75" s="28" t="n">
         <v>0.02</v>
       </c>
-      <c r="D75" s="27" t="n">
+      <c r="D75" s="28" t="n">
         <v>0.013</v>
       </c>
-      <c r="E75" s="27" t="n">
+      <c r="E75" s="28" t="n">
         <v>0.029</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B76" s="25" t="s">
-        <v>110</v>
-      </c>
-      <c r="C76" s="27" t="n">
+      <c r="B76" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="C76" s="28" t="n">
         <v>0.07</v>
       </c>
-      <c r="D76" s="27" t="n">
+      <c r="D76" s="28" t="n">
         <v>0.048</v>
       </c>
-      <c r="E76" s="27" t="n">
+      <c r="E76" s="28" t="n">
         <v>0.094</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B77" s="25" t="s">
-        <v>111</v>
-      </c>
-      <c r="C77" s="27" t="n">
+      <c r="B77" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="C77" s="28" t="n">
         <v>0.265</v>
       </c>
-      <c r="D77" s="27" t="n">
+      <c r="D77" s="28" t="n">
         <v>0.114</v>
       </c>
-      <c r="E77" s="27" t="n">
+      <c r="E77" s="28" t="n">
         <v>0.474</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B78" s="25" t="s">
-        <v>112</v>
-      </c>
-      <c r="C78" s="27" t="n">
+      <c r="B78" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="C78" s="28" t="n">
         <v>0.547</v>
       </c>
-      <c r="D78" s="27" t="n">
+      <c r="D78" s="28" t="n">
         <v>0.382</v>
       </c>
-      <c r="E78" s="27" t="n">
+      <c r="E78" s="28" t="n">
         <v>0.715</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B79" s="25" t="s">
-        <v>113</v>
-      </c>
-      <c r="C79" s="27" t="n">
+      <c r="B79" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="C79" s="28" t="n">
         <v>0.053</v>
       </c>
-      <c r="D79" s="27" t="n">
+      <c r="D79" s="28" t="n">
         <v>0.034</v>
       </c>
-      <c r="E79" s="27" t="n">
+      <c r="E79" s="28" t="n">
         <v>0.079</v>
       </c>
     </row>
@@ -3536,12 +3553,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.6989795918367"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.2091836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="55.1683673469388"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="11.6989795918367"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.9744897959184"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.86224489795918"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="22.5867346938776"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.9744897959184"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="110.780612244898"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="22.5867346938776"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="33.6020408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="19.265306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3660,8 +3677,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="36" min="1" style="0" width="11.6989795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="37" style="0" width="9.86224489795918"/>
+    <col collapsed="false" hidden="false" max="36" min="1" style="0" width="22.5867346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="37" style="0" width="19.265306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4066,14 +4083,14 @@
   </sheetPr>
   <dimension ref="A1:AJ9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B17" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L8" activeCellId="0" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="36" min="1" style="0" width="11.6989795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="37" style="0" width="9.86224489795918"/>
+    <col collapsed="false" hidden="false" max="36" min="1" style="0" width="22.5867346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="37" style="0" width="19.265306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4480,8 +4497,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="35" min="1" style="0" width="11.6989795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="36" style="0" width="9.86224489795918"/>
+    <col collapsed="false" hidden="false" max="35" min="1" style="0" width="22.5867346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="36" style="0" width="19.265306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5081,8 +5098,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="35" min="1" style="0" width="11.6989795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="36" style="0" width="9.86224489795918"/>
+    <col collapsed="false" hidden="false" max="35" min="1" style="0" width="22.5867346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="36" style="0" width="19.265306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6102,15 +6119,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AI65536"/>
+  <dimension ref="A1:AI68"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AI38" activeCellId="0" sqref="AI38"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AI19" activeCellId="0" sqref="AI19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.86224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="19.265306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6256,7 +6273,7 @@
         <v>21</v>
       </c>
       <c r="AI3" s="18" t="n">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6299,7 +6316,7 @@
         <v>21</v>
       </c>
       <c r="AI4" s="18" t="n">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6445,7 +6462,7 @@
         <v>21</v>
       </c>
       <c r="AI10" s="18" t="n">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6488,9 +6505,10 @@
         <v>21</v>
       </c>
       <c r="AI11" s="18" t="n">
-        <v>0.6</v>
-      </c>
-    </row>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="15" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="15" t="s">
         <v>38</v>
@@ -6634,7 +6652,7 @@
         <v>21</v>
       </c>
       <c r="AI17" s="18" t="n">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6677,7 +6695,7 @@
         <v>21</v>
       </c>
       <c r="AI18" s="18" t="n">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6823,7 +6841,7 @@
         <v>21</v>
       </c>
       <c r="AI24" s="18" t="n">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6866,9 +6884,10 @@
         <v>21</v>
       </c>
       <c r="AI25" s="18" t="n">
-        <v>0.3</v>
-      </c>
-    </row>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="15" t="s">
@@ -7012,7 +7031,7 @@
         <v>21</v>
       </c>
       <c r="AI31" s="18" t="n">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -7160,11 +7179,12 @@
         <v>21</v>
       </c>
       <c r="AI37" s="18" t="n">
-        <v>0.9</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="15" t="s">
         <v>43</v>
@@ -7306,20 +7326,611 @@
       <c r="AH43" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="AI43" s="18" t="n">
-        <v>0.1</v>
+      <c r="AI43" s="19" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C48" s="16" t="n">
+        <v>2000</v>
+      </c>
+      <c r="D48" s="16" t="n">
+        <v>2001</v>
+      </c>
+      <c r="E48" s="16" t="n">
+        <v>2002</v>
+      </c>
+      <c r="F48" s="16" t="n">
+        <v>2003</v>
+      </c>
+      <c r="G48" s="16" t="n">
+        <v>2004</v>
+      </c>
+      <c r="H48" s="16" t="n">
+        <v>2005</v>
+      </c>
+      <c r="I48" s="16" t="n">
+        <v>2006</v>
+      </c>
+      <c r="J48" s="16" t="n">
+        <v>2007</v>
+      </c>
+      <c r="K48" s="16" t="n">
+        <v>2008</v>
+      </c>
+      <c r="L48" s="16" t="n">
+        <v>2009</v>
+      </c>
+      <c r="M48" s="16" t="n">
+        <v>2010</v>
+      </c>
+      <c r="N48" s="16" t="n">
+        <v>2011</v>
+      </c>
+      <c r="O48" s="16" t="n">
+        <v>2012</v>
+      </c>
+      <c r="P48" s="16" t="n">
+        <v>2013</v>
+      </c>
+      <c r="Q48" s="16" t="n">
+        <v>2014</v>
+      </c>
+      <c r="R48" s="16" t="n">
+        <v>2015</v>
+      </c>
+      <c r="S48" s="16" t="n">
+        <v>2016</v>
+      </c>
+      <c r="T48" s="16" t="n">
+        <v>2017</v>
+      </c>
+      <c r="U48" s="16" t="n">
+        <v>2018</v>
+      </c>
+      <c r="V48" s="16" t="n">
+        <v>2019</v>
+      </c>
+      <c r="W48" s="16" t="n">
+        <v>2020</v>
+      </c>
+      <c r="X48" s="16" t="n">
+        <v>2021</v>
+      </c>
+      <c r="Y48" s="16" t="n">
+        <v>2022</v>
+      </c>
+      <c r="Z48" s="16" t="n">
+        <v>2023</v>
+      </c>
+      <c r="AA48" s="16" t="n">
+        <v>2024</v>
+      </c>
+      <c r="AB48" s="16" t="n">
+        <v>2025</v>
+      </c>
+      <c r="AC48" s="16" t="n">
+        <v>2026</v>
+      </c>
+      <c r="AD48" s="16" t="n">
+        <v>2027</v>
+      </c>
+      <c r="AE48" s="16" t="n">
+        <v>2028</v>
+      </c>
+      <c r="AF48" s="16" t="n">
+        <v>2029</v>
+      </c>
+      <c r="AG48" s="16" t="n">
+        <v>2030</v>
+      </c>
+      <c r="AI48" s="16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B49" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C49" s="18"/>
+      <c r="D49" s="18"/>
+      <c r="E49" s="18"/>
+      <c r="F49" s="18"/>
+      <c r="G49" s="18"/>
+      <c r="H49" s="18"/>
+      <c r="I49" s="18"/>
+      <c r="J49" s="18"/>
+      <c r="K49" s="18"/>
+      <c r="L49" s="18"/>
+      <c r="M49" s="18"/>
+      <c r="N49" s="18"/>
+      <c r="O49" s="18"/>
+      <c r="P49" s="18"/>
+      <c r="Q49" s="18"/>
+      <c r="R49" s="18"/>
+      <c r="S49" s="18"/>
+      <c r="T49" s="18"/>
+      <c r="U49" s="18"/>
+      <c r="V49" s="18"/>
+      <c r="W49" s="18"/>
+      <c r="X49" s="18"/>
+      <c r="Y49" s="18"/>
+      <c r="Z49" s="18"/>
+      <c r="AA49" s="18"/>
+      <c r="AB49" s="18"/>
+      <c r="AC49" s="18"/>
+      <c r="AD49" s="18"/>
+      <c r="AE49" s="18"/>
+      <c r="AF49" s="18"/>
+      <c r="AG49" s="18"/>
+      <c r="AH49" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="AI49" s="19" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C54" s="16" t="n">
+        <v>2000</v>
+      </c>
+      <c r="D54" s="16" t="n">
+        <v>2001</v>
+      </c>
+      <c r="E54" s="16" t="n">
+        <v>2002</v>
+      </c>
+      <c r="F54" s="16" t="n">
+        <v>2003</v>
+      </c>
+      <c r="G54" s="16" t="n">
+        <v>2004</v>
+      </c>
+      <c r="H54" s="16" t="n">
+        <v>2005</v>
+      </c>
+      <c r="I54" s="16" t="n">
+        <v>2006</v>
+      </c>
+      <c r="J54" s="16" t="n">
+        <v>2007</v>
+      </c>
+      <c r="K54" s="16" t="n">
+        <v>2008</v>
+      </c>
+      <c r="L54" s="16" t="n">
+        <v>2009</v>
+      </c>
+      <c r="M54" s="16" t="n">
+        <v>2010</v>
+      </c>
+      <c r="N54" s="16" t="n">
+        <v>2011</v>
+      </c>
+      <c r="O54" s="16" t="n">
+        <v>2012</v>
+      </c>
+      <c r="P54" s="16" t="n">
+        <v>2013</v>
+      </c>
+      <c r="Q54" s="16" t="n">
+        <v>2014</v>
+      </c>
+      <c r="R54" s="16" t="n">
+        <v>2015</v>
+      </c>
+      <c r="S54" s="16" t="n">
+        <v>2016</v>
+      </c>
+      <c r="T54" s="16" t="n">
+        <v>2017</v>
+      </c>
+      <c r="U54" s="16" t="n">
+        <v>2018</v>
+      </c>
+      <c r="V54" s="16" t="n">
+        <v>2019</v>
+      </c>
+      <c r="W54" s="16" t="n">
+        <v>2020</v>
+      </c>
+      <c r="X54" s="16" t="n">
+        <v>2021</v>
+      </c>
+      <c r="Y54" s="16" t="n">
+        <v>2022</v>
+      </c>
+      <c r="Z54" s="16" t="n">
+        <v>2023</v>
+      </c>
+      <c r="AA54" s="16" t="n">
+        <v>2024</v>
+      </c>
+      <c r="AB54" s="16" t="n">
+        <v>2025</v>
+      </c>
+      <c r="AC54" s="16" t="n">
+        <v>2026</v>
+      </c>
+      <c r="AD54" s="16" t="n">
+        <v>2027</v>
+      </c>
+      <c r="AE54" s="16" t="n">
+        <v>2028</v>
+      </c>
+      <c r="AF54" s="16" t="n">
+        <v>2029</v>
+      </c>
+      <c r="AG54" s="16" t="n">
+        <v>2030</v>
+      </c>
+      <c r="AI54" s="16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B55" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C55" s="18"/>
+      <c r="D55" s="18"/>
+      <c r="E55" s="18"/>
+      <c r="F55" s="18"/>
+      <c r="G55" s="18"/>
+      <c r="H55" s="18"/>
+      <c r="I55" s="18"/>
+      <c r="J55" s="18"/>
+      <c r="K55" s="18"/>
+      <c r="L55" s="18"/>
+      <c r="M55" s="18"/>
+      <c r="N55" s="18"/>
+      <c r="O55" s="18"/>
+      <c r="P55" s="18"/>
+      <c r="Q55" s="18"/>
+      <c r="R55" s="18"/>
+      <c r="S55" s="18"/>
+      <c r="T55" s="18"/>
+      <c r="U55" s="18"/>
+      <c r="V55" s="18"/>
+      <c r="W55" s="18"/>
+      <c r="X55" s="18"/>
+      <c r="Y55" s="18"/>
+      <c r="Z55" s="18"/>
+      <c r="AA55" s="18"/>
+      <c r="AB55" s="18"/>
+      <c r="AC55" s="18"/>
+      <c r="AD55" s="18"/>
+      <c r="AE55" s="18"/>
+      <c r="AF55" s="18"/>
+      <c r="AG55" s="18"/>
+      <c r="AH55" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="AI55" s="18" t="n">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C60" s="16" t="n">
+        <v>2000</v>
+      </c>
+      <c r="D60" s="16" t="n">
+        <v>2001</v>
+      </c>
+      <c r="E60" s="16" t="n">
+        <v>2002</v>
+      </c>
+      <c r="F60" s="16" t="n">
+        <v>2003</v>
+      </c>
+      <c r="G60" s="16" t="n">
+        <v>2004</v>
+      </c>
+      <c r="H60" s="16" t="n">
+        <v>2005</v>
+      </c>
+      <c r="I60" s="16" t="n">
+        <v>2006</v>
+      </c>
+      <c r="J60" s="16" t="n">
+        <v>2007</v>
+      </c>
+      <c r="K60" s="16" t="n">
+        <v>2008</v>
+      </c>
+      <c r="L60" s="16" t="n">
+        <v>2009</v>
+      </c>
+      <c r="M60" s="16" t="n">
+        <v>2010</v>
+      </c>
+      <c r="N60" s="16" t="n">
+        <v>2011</v>
+      </c>
+      <c r="O60" s="16" t="n">
+        <v>2012</v>
+      </c>
+      <c r="P60" s="16" t="n">
+        <v>2013</v>
+      </c>
+      <c r="Q60" s="16" t="n">
+        <v>2014</v>
+      </c>
+      <c r="R60" s="16" t="n">
+        <v>2015</v>
+      </c>
+      <c r="S60" s="16" t="n">
+        <v>2016</v>
+      </c>
+      <c r="T60" s="16" t="n">
+        <v>2017</v>
+      </c>
+      <c r="U60" s="16" t="n">
+        <v>2018</v>
+      </c>
+      <c r="V60" s="16" t="n">
+        <v>2019</v>
+      </c>
+      <c r="W60" s="16" t="n">
+        <v>2020</v>
+      </c>
+      <c r="X60" s="16" t="n">
+        <v>2021</v>
+      </c>
+      <c r="Y60" s="16" t="n">
+        <v>2022</v>
+      </c>
+      <c r="Z60" s="16" t="n">
+        <v>2023</v>
+      </c>
+      <c r="AA60" s="16" t="n">
+        <v>2024</v>
+      </c>
+      <c r="AB60" s="16" t="n">
+        <v>2025</v>
+      </c>
+      <c r="AC60" s="16" t="n">
+        <v>2026</v>
+      </c>
+      <c r="AD60" s="16" t="n">
+        <v>2027</v>
+      </c>
+      <c r="AE60" s="16" t="n">
+        <v>2028</v>
+      </c>
+      <c r="AF60" s="16" t="n">
+        <v>2029</v>
+      </c>
+      <c r="AG60" s="16" t="n">
+        <v>2030</v>
+      </c>
+      <c r="AI60" s="16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B61" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C61" s="18"/>
+      <c r="D61" s="18"/>
+      <c r="E61" s="18"/>
+      <c r="F61" s="18"/>
+      <c r="G61" s="18"/>
+      <c r="H61" s="18"/>
+      <c r="I61" s="18"/>
+      <c r="J61" s="18"/>
+      <c r="K61" s="18"/>
+      <c r="L61" s="18"/>
+      <c r="M61" s="18"/>
+      <c r="N61" s="18"/>
+      <c r="O61" s="18"/>
+      <c r="P61" s="18"/>
+      <c r="Q61" s="18"/>
+      <c r="R61" s="18"/>
+      <c r="S61" s="18"/>
+      <c r="T61" s="18"/>
+      <c r="U61" s="18"/>
+      <c r="V61" s="18"/>
+      <c r="W61" s="18"/>
+      <c r="X61" s="18"/>
+      <c r="Y61" s="18"/>
+      <c r="Z61" s="18"/>
+      <c r="AA61" s="18"/>
+      <c r="AB61" s="18"/>
+      <c r="AC61" s="18"/>
+      <c r="AD61" s="18"/>
+      <c r="AE61" s="18"/>
+      <c r="AF61" s="18"/>
+      <c r="AG61" s="18"/>
+      <c r="AH61" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="AI61" s="18" t="n">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C66" s="16" t="n">
+        <v>2000</v>
+      </c>
+      <c r="D66" s="16" t="n">
+        <v>2001</v>
+      </c>
+      <c r="E66" s="16" t="n">
+        <v>2002</v>
+      </c>
+      <c r="F66" s="16" t="n">
+        <v>2003</v>
+      </c>
+      <c r="G66" s="16" t="n">
+        <v>2004</v>
+      </c>
+      <c r="H66" s="16" t="n">
+        <v>2005</v>
+      </c>
+      <c r="I66" s="16" t="n">
+        <v>2006</v>
+      </c>
+      <c r="J66" s="16" t="n">
+        <v>2007</v>
+      </c>
+      <c r="K66" s="16" t="n">
+        <v>2008</v>
+      </c>
+      <c r="L66" s="16" t="n">
+        <v>2009</v>
+      </c>
+      <c r="M66" s="16" t="n">
+        <v>2010</v>
+      </c>
+      <c r="N66" s="16" t="n">
+        <v>2011</v>
+      </c>
+      <c r="O66" s="16" t="n">
+        <v>2012</v>
+      </c>
+      <c r="P66" s="16" t="n">
+        <v>2013</v>
+      </c>
+      <c r="Q66" s="16" t="n">
+        <v>2014</v>
+      </c>
+      <c r="R66" s="16" t="n">
+        <v>2015</v>
+      </c>
+      <c r="S66" s="16" t="n">
+        <v>2016</v>
+      </c>
+      <c r="T66" s="16" t="n">
+        <v>2017</v>
+      </c>
+      <c r="U66" s="16" t="n">
+        <v>2018</v>
+      </c>
+      <c r="V66" s="16" t="n">
+        <v>2019</v>
+      </c>
+      <c r="W66" s="16" t="n">
+        <v>2020</v>
+      </c>
+      <c r="X66" s="16" t="n">
+        <v>2021</v>
+      </c>
+      <c r="Y66" s="16" t="n">
+        <v>2022</v>
+      </c>
+      <c r="Z66" s="16" t="n">
+        <v>2023</v>
+      </c>
+      <c r="AA66" s="16" t="n">
+        <v>2024</v>
+      </c>
+      <c r="AB66" s="16" t="n">
+        <v>2025</v>
+      </c>
+      <c r="AC66" s="16" t="n">
+        <v>2026</v>
+      </c>
+      <c r="AD66" s="16" t="n">
+        <v>2027</v>
+      </c>
+      <c r="AE66" s="16" t="n">
+        <v>2028</v>
+      </c>
+      <c r="AF66" s="16" t="n">
+        <v>2029</v>
+      </c>
+      <c r="AG66" s="16" t="n">
+        <v>2030</v>
+      </c>
+      <c r="AI66" s="16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B67" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C67" s="18"/>
+      <c r="D67" s="18"/>
+      <c r="E67" s="18"/>
+      <c r="F67" s="18"/>
+      <c r="G67" s="18"/>
+      <c r="H67" s="18"/>
+      <c r="I67" s="18"/>
+      <c r="J67" s="18"/>
+      <c r="K67" s="18"/>
+      <c r="L67" s="18"/>
+      <c r="M67" s="18"/>
+      <c r="N67" s="18"/>
+      <c r="O67" s="18"/>
+      <c r="P67" s="18"/>
+      <c r="Q67" s="18"/>
+      <c r="R67" s="18"/>
+      <c r="S67" s="18"/>
+      <c r="T67" s="18"/>
+      <c r="U67" s="18"/>
+      <c r="V67" s="18"/>
+      <c r="W67" s="18"/>
+      <c r="X67" s="18"/>
+      <c r="Y67" s="18"/>
+      <c r="Z67" s="18"/>
+      <c r="AA67" s="18"/>
+      <c r="AB67" s="18"/>
+      <c r="AC67" s="18"/>
+      <c r="AD67" s="18"/>
+      <c r="AE67" s="18"/>
+      <c r="AF67" s="18"/>
+      <c r="AG67" s="18"/>
+      <c r="AH67" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="AI67" s="18" t="n">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -7338,19 +7949,19 @@
   </sheetPr>
   <dimension ref="A1:AI41"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J17" activeCellId="0" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="35" min="1" style="0" width="11.6989795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="36" style="0" width="9.86224489795918"/>
+    <col collapsed="false" hidden="false" max="35" min="1" style="0" width="22.5867346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="36" style="0" width="19.265306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7456,90 +8067,90 @@
         <f aca="false">Populations!$C$3</f>
         <v>M 15-49</v>
       </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19"/>
-      <c r="M3" s="19" t="n">
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20" t="n">
         <v>0.0645</v>
       </c>
-      <c r="N3" s="19"/>
-      <c r="O3" s="19"/>
-      <c r="P3" s="19"/>
-      <c r="Q3" s="19"/>
-      <c r="R3" s="19"/>
-      <c r="S3" s="19"/>
-      <c r="T3" s="19"/>
-      <c r="U3" s="19"/>
-      <c r="V3" s="19"/>
-      <c r="W3" s="19"/>
-      <c r="X3" s="19"/>
-      <c r="Y3" s="19"/>
-      <c r="Z3" s="19"/>
-      <c r="AA3" s="19"/>
-      <c r="AB3" s="19"/>
-      <c r="AC3" s="19"/>
-      <c r="AD3" s="19"/>
-      <c r="AE3" s="19"/>
-      <c r="AF3" s="19"/>
-      <c r="AG3" s="19"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="20"/>
+      <c r="P3" s="20"/>
+      <c r="Q3" s="20"/>
+      <c r="R3" s="20"/>
+      <c r="S3" s="20"/>
+      <c r="T3" s="20"/>
+      <c r="U3" s="20"/>
+      <c r="V3" s="20"/>
+      <c r="W3" s="20"/>
+      <c r="X3" s="20"/>
+      <c r="Y3" s="20"/>
+      <c r="Z3" s="20"/>
+      <c r="AA3" s="20"/>
+      <c r="AB3" s="20"/>
+      <c r="AC3" s="20"/>
+      <c r="AD3" s="20"/>
+      <c r="AE3" s="20"/>
+      <c r="AF3" s="20"/>
+      <c r="AG3" s="20"/>
       <c r="AH3" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="AI3" s="19"/>
+      <c r="AI3" s="20"/>
     </row>
     <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="6" t="str">
         <f aca="false">Populations!$C$4</f>
         <v>F 15-49</v>
       </c>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="19" t="n">
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20" t="n">
         <v>0.0645</v>
       </c>
-      <c r="N4" s="19"/>
-      <c r="O4" s="19"/>
-      <c r="P4" s="19"/>
-      <c r="Q4" s="19"/>
-      <c r="R4" s="19"/>
-      <c r="S4" s="19"/>
-      <c r="T4" s="19"/>
-      <c r="U4" s="19"/>
-      <c r="V4" s="19"/>
-      <c r="W4" s="19"/>
-      <c r="X4" s="19"/>
-      <c r="Y4" s="19"/>
-      <c r="Z4" s="19"/>
-      <c r="AA4" s="19"/>
-      <c r="AB4" s="19"/>
-      <c r="AC4" s="19"/>
-      <c r="AD4" s="19"/>
-      <c r="AE4" s="19"/>
-      <c r="AF4" s="19"/>
-      <c r="AG4" s="19"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="20"/>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="20"/>
+      <c r="S4" s="20"/>
+      <c r="T4" s="20"/>
+      <c r="U4" s="20"/>
+      <c r="V4" s="20"/>
+      <c r="W4" s="20"/>
+      <c r="X4" s="20"/>
+      <c r="Y4" s="20"/>
+      <c r="Z4" s="20"/>
+      <c r="AA4" s="20"/>
+      <c r="AB4" s="20"/>
+      <c r="AC4" s="20"/>
+      <c r="AD4" s="20"/>
+      <c r="AE4" s="20"/>
+      <c r="AF4" s="20"/>
+      <c r="AG4" s="20"/>
       <c r="AH4" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="AI4" s="19"/>
+      <c r="AI4" s="20"/>
     </row>
     <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7678,13 +8289,13 @@
       <c r="AH10" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="AI10" s="20" t="n">
+      <c r="AI10" s="21" t="n">
         <v>0.65</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7796,12 +8407,14 @@
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7" t="n">
-        <v>50</v>
-      </c>
-      <c r="H16" s="7"/>
+        <v>100</v>
+      </c>
+      <c r="H16" s="7" t="n">
+        <v>400</v>
+      </c>
       <c r="I16" s="7"/>
       <c r="J16" s="7" t="n">
-        <v>600</v>
+        <v>1200</v>
       </c>
       <c r="K16" s="7"/>
       <c r="L16" s="7"/>
@@ -7837,7 +8450,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7943,90 +8556,90 @@
         <f aca="false">Populations!$C$3</f>
         <v>M 15-49</v>
       </c>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="19"/>
-      <c r="J22" s="19"/>
-      <c r="K22" s="19"/>
-      <c r="L22" s="19"/>
-      <c r="M22" s="19"/>
-      <c r="N22" s="19"/>
-      <c r="O22" s="19"/>
-      <c r="P22" s="19"/>
-      <c r="Q22" s="19" t="n">
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="20"/>
+      <c r="L22" s="20"/>
+      <c r="M22" s="20"/>
+      <c r="N22" s="20"/>
+      <c r="O22" s="20"/>
+      <c r="P22" s="20"/>
+      <c r="Q22" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="R22" s="19"/>
-      <c r="S22" s="19"/>
-      <c r="T22" s="19"/>
-      <c r="U22" s="19"/>
-      <c r="V22" s="19"/>
-      <c r="W22" s="19"/>
-      <c r="X22" s="19"/>
-      <c r="Y22" s="19"/>
-      <c r="Z22" s="19"/>
-      <c r="AA22" s="19"/>
-      <c r="AB22" s="19"/>
-      <c r="AC22" s="19"/>
-      <c r="AD22" s="19"/>
-      <c r="AE22" s="19"/>
-      <c r="AF22" s="19"/>
-      <c r="AG22" s="19"/>
+      <c r="R22" s="20"/>
+      <c r="S22" s="20"/>
+      <c r="T22" s="20"/>
+      <c r="U22" s="20"/>
+      <c r="V22" s="20"/>
+      <c r="W22" s="20"/>
+      <c r="X22" s="20"/>
+      <c r="Y22" s="20"/>
+      <c r="Z22" s="20"/>
+      <c r="AA22" s="20"/>
+      <c r="AB22" s="20"/>
+      <c r="AC22" s="20"/>
+      <c r="AD22" s="20"/>
+      <c r="AE22" s="20"/>
+      <c r="AF22" s="20"/>
+      <c r="AG22" s="20"/>
       <c r="AH22" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="AI22" s="19"/>
+      <c r="AI22" s="20"/>
     </row>
     <row r="23" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B23" s="6" t="str">
         <f aca="false">Populations!$C$4</f>
         <v>F 15-49</v>
       </c>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="19"/>
-      <c r="J23" s="19"/>
-      <c r="K23" s="19"/>
-      <c r="L23" s="19"/>
-      <c r="M23" s="19"/>
-      <c r="N23" s="19"/>
-      <c r="O23" s="19"/>
-      <c r="P23" s="19"/>
-      <c r="Q23" s="19" t="n">
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="20"/>
+      <c r="L23" s="20"/>
+      <c r="M23" s="20"/>
+      <c r="N23" s="20"/>
+      <c r="O23" s="20"/>
+      <c r="P23" s="20"/>
+      <c r="Q23" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="R23" s="19"/>
-      <c r="S23" s="19"/>
-      <c r="T23" s="19"/>
-      <c r="U23" s="19"/>
-      <c r="V23" s="19"/>
-      <c r="W23" s="19"/>
-      <c r="X23" s="19"/>
-      <c r="Y23" s="19"/>
-      <c r="Z23" s="19"/>
-      <c r="AA23" s="19"/>
-      <c r="AB23" s="19"/>
-      <c r="AC23" s="19"/>
-      <c r="AD23" s="19"/>
-      <c r="AE23" s="19"/>
-      <c r="AF23" s="19"/>
-      <c r="AG23" s="19"/>
+      <c r="R23" s="20"/>
+      <c r="S23" s="20"/>
+      <c r="T23" s="20"/>
+      <c r="U23" s="20"/>
+      <c r="V23" s="20"/>
+      <c r="W23" s="20"/>
+      <c r="X23" s="20"/>
+      <c r="Y23" s="20"/>
+      <c r="Z23" s="20"/>
+      <c r="AA23" s="20"/>
+      <c r="AB23" s="20"/>
+      <c r="AC23" s="20"/>
+      <c r="AD23" s="20"/>
+      <c r="AE23" s="20"/>
+      <c r="AF23" s="20"/>
+      <c r="AG23" s="20"/>
       <c r="AH23" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="AI23" s="19"/>
+      <c r="AI23" s="20"/>
     </row>
     <row r="27" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8179,7 +8792,7 @@
     </row>
     <row r="33" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8349,7 +8962,7 @@
     </row>
     <row r="39" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="3" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8454,41 +9067,41 @@
       <c r="B41" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C41" s="19"/>
-      <c r="D41" s="19"/>
-      <c r="E41" s="19"/>
-      <c r="F41" s="19"/>
-      <c r="G41" s="19"/>
-      <c r="H41" s="19"/>
-      <c r="I41" s="19"/>
-      <c r="J41" s="19"/>
-      <c r="K41" s="19"/>
-      <c r="L41" s="19"/>
-      <c r="M41" s="19"/>
-      <c r="N41" s="19"/>
-      <c r="O41" s="19"/>
-      <c r="P41" s="19"/>
-      <c r="Q41" s="19"/>
-      <c r="R41" s="19"/>
-      <c r="S41" s="19"/>
-      <c r="T41" s="19"/>
-      <c r="U41" s="19"/>
-      <c r="V41" s="19"/>
-      <c r="W41" s="19"/>
-      <c r="X41" s="19"/>
-      <c r="Y41" s="19"/>
-      <c r="Z41" s="19"/>
-      <c r="AA41" s="19"/>
-      <c r="AB41" s="19"/>
-      <c r="AC41" s="19"/>
-      <c r="AD41" s="19"/>
-      <c r="AE41" s="19"/>
-      <c r="AF41" s="19"/>
-      <c r="AG41" s="19"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="20"/>
+      <c r="F41" s="20"/>
+      <c r="G41" s="20"/>
+      <c r="H41" s="20"/>
+      <c r="I41" s="20"/>
+      <c r="J41" s="20"/>
+      <c r="K41" s="20"/>
+      <c r="L41" s="20"/>
+      <c r="M41" s="20"/>
+      <c r="N41" s="20"/>
+      <c r="O41" s="20"/>
+      <c r="P41" s="20"/>
+      <c r="Q41" s="20"/>
+      <c r="R41" s="20"/>
+      <c r="S41" s="20"/>
+      <c r="T41" s="20"/>
+      <c r="U41" s="20"/>
+      <c r="V41" s="20"/>
+      <c r="W41" s="20"/>
+      <c r="X41" s="20"/>
+      <c r="Y41" s="20"/>
+      <c r="Z41" s="20"/>
+      <c r="AA41" s="20"/>
+      <c r="AB41" s="20"/>
+      <c r="AC41" s="20"/>
+      <c r="AD41" s="20"/>
+      <c r="AE41" s="20"/>
+      <c r="AF41" s="20"/>
+      <c r="AG41" s="20"/>
       <c r="AH41" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="AI41" s="21" t="n">
+      <c r="AI41" s="22" t="n">
         <f aca="false">14/100*87/100</f>
         <v>0.1218</v>
       </c>
@@ -8519,13 +9132,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="35" min="1" style="0" width="11.6989795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="36" style="0" width="9.86224489795918"/>
+    <col collapsed="false" hidden="false" max="35" min="1" style="0" width="22.5867346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="36" style="0" width="19.265306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8665,7 +9278,7 @@
       <c r="AH3" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="AI3" s="22" t="n">
+      <c r="AI3" s="23" t="n">
         <v>100</v>
       </c>
     </row>
@@ -8708,13 +9321,13 @@
       <c r="AH4" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="AI4" s="22" t="n">
+      <c r="AI4" s="23" t="n">
         <v>100</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8854,7 +9467,7 @@
       <c r="AH10" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="AI10" s="22" t="n">
+      <c r="AI10" s="23" t="n">
         <f aca="false">0.2*3*20</f>
         <v>12</v>
       </c>
@@ -8898,14 +9511,14 @@
       <c r="AH11" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="AI11" s="22" t="n">
+      <c r="AI11" s="23" t="n">
         <f aca="false">0.1*3*20</f>
         <v>6</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9094,7 +9707,7 @@
     </row>
     <row r="22" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9200,41 +9813,41 @@
         <f aca="false">Populations!$C$3</f>
         <v>M 15-49</v>
       </c>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="19"/>
-      <c r="I24" s="19"/>
-      <c r="J24" s="19"/>
-      <c r="K24" s="19"/>
-      <c r="L24" s="19"/>
-      <c r="M24" s="19"/>
-      <c r="N24" s="19"/>
-      <c r="O24" s="19"/>
-      <c r="P24" s="19"/>
-      <c r="Q24" s="19"/>
-      <c r="R24" s="19"/>
-      <c r="S24" s="19"/>
-      <c r="T24" s="19"/>
-      <c r="U24" s="19"/>
-      <c r="V24" s="19"/>
-      <c r="W24" s="19"/>
-      <c r="X24" s="19"/>
-      <c r="Y24" s="19"/>
-      <c r="Z24" s="19"/>
-      <c r="AA24" s="19"/>
-      <c r="AB24" s="19"/>
-      <c r="AC24" s="19"/>
-      <c r="AD24" s="19"/>
-      <c r="AE24" s="19"/>
-      <c r="AF24" s="19"/>
-      <c r="AG24" s="19"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="20"/>
+      <c r="K24" s="20"/>
+      <c r="L24" s="20"/>
+      <c r="M24" s="20"/>
+      <c r="N24" s="20"/>
+      <c r="O24" s="20"/>
+      <c r="P24" s="20"/>
+      <c r="Q24" s="20"/>
+      <c r="R24" s="20"/>
+      <c r="S24" s="20"/>
+      <c r="T24" s="20"/>
+      <c r="U24" s="20"/>
+      <c r="V24" s="20"/>
+      <c r="W24" s="20"/>
+      <c r="X24" s="20"/>
+      <c r="Y24" s="20"/>
+      <c r="Z24" s="20"/>
+      <c r="AA24" s="20"/>
+      <c r="AB24" s="20"/>
+      <c r="AC24" s="20"/>
+      <c r="AD24" s="20"/>
+      <c r="AE24" s="20"/>
+      <c r="AF24" s="20"/>
+      <c r="AG24" s="20"/>
       <c r="AH24" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="AI24" s="23" t="n">
+      <c r="AI24" s="24" t="n">
         <v>0.14</v>
       </c>
     </row>
@@ -9243,47 +9856,47 @@
         <f aca="false">Populations!$C$4</f>
         <v>F 15-49</v>
       </c>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="19"/>
-      <c r="J25" s="19"/>
-      <c r="K25" s="19"/>
-      <c r="L25" s="19"/>
-      <c r="M25" s="19"/>
-      <c r="N25" s="19"/>
-      <c r="O25" s="19"/>
-      <c r="P25" s="19"/>
-      <c r="Q25" s="19"/>
-      <c r="R25" s="19"/>
-      <c r="S25" s="19"/>
-      <c r="T25" s="19"/>
-      <c r="U25" s="19"/>
-      <c r="V25" s="19"/>
-      <c r="W25" s="19"/>
-      <c r="X25" s="19"/>
-      <c r="Y25" s="19"/>
-      <c r="Z25" s="19"/>
-      <c r="AA25" s="19"/>
-      <c r="AB25" s="19"/>
-      <c r="AC25" s="19"/>
-      <c r="AD25" s="19"/>
-      <c r="AE25" s="19"/>
-      <c r="AF25" s="19"/>
-      <c r="AG25" s="19"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="20"/>
+      <c r="L25" s="20"/>
+      <c r="M25" s="20"/>
+      <c r="N25" s="20"/>
+      <c r="O25" s="20"/>
+      <c r="P25" s="20"/>
+      <c r="Q25" s="20"/>
+      <c r="R25" s="20"/>
+      <c r="S25" s="20"/>
+      <c r="T25" s="20"/>
+      <c r="U25" s="20"/>
+      <c r="V25" s="20"/>
+      <c r="W25" s="20"/>
+      <c r="X25" s="20"/>
+      <c r="Y25" s="20"/>
+      <c r="Z25" s="20"/>
+      <c r="AA25" s="20"/>
+      <c r="AB25" s="20"/>
+      <c r="AC25" s="20"/>
+      <c r="AD25" s="20"/>
+      <c r="AE25" s="20"/>
+      <c r="AF25" s="20"/>
+      <c r="AG25" s="20"/>
       <c r="AH25" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="AI25" s="23" t="n">
+      <c r="AI25" s="24" t="n">
         <v>0.14</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9389,41 +10002,41 @@
         <f aca="false">Populations!$C$3</f>
         <v>M 15-49</v>
       </c>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="19"/>
-      <c r="H31" s="19"/>
-      <c r="I31" s="19"/>
-      <c r="J31" s="19"/>
-      <c r="K31" s="19"/>
-      <c r="L31" s="19"/>
-      <c r="M31" s="19"/>
-      <c r="N31" s="19"/>
-      <c r="O31" s="19"/>
-      <c r="P31" s="19"/>
-      <c r="Q31" s="19"/>
-      <c r="R31" s="19"/>
-      <c r="S31" s="19"/>
-      <c r="T31" s="19"/>
-      <c r="U31" s="19"/>
-      <c r="V31" s="19"/>
-      <c r="W31" s="19"/>
-      <c r="X31" s="19"/>
-      <c r="Y31" s="19"/>
-      <c r="Z31" s="19"/>
-      <c r="AA31" s="19"/>
-      <c r="AB31" s="19"/>
-      <c r="AC31" s="19"/>
-      <c r="AD31" s="19"/>
-      <c r="AE31" s="19"/>
-      <c r="AF31" s="19"/>
-      <c r="AG31" s="19"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="20"/>
+      <c r="J31" s="20"/>
+      <c r="K31" s="20"/>
+      <c r="L31" s="20"/>
+      <c r="M31" s="20"/>
+      <c r="N31" s="20"/>
+      <c r="O31" s="20"/>
+      <c r="P31" s="20"/>
+      <c r="Q31" s="20"/>
+      <c r="R31" s="20"/>
+      <c r="S31" s="20"/>
+      <c r="T31" s="20"/>
+      <c r="U31" s="20"/>
+      <c r="V31" s="20"/>
+      <c r="W31" s="20"/>
+      <c r="X31" s="20"/>
+      <c r="Y31" s="20"/>
+      <c r="Z31" s="20"/>
+      <c r="AA31" s="20"/>
+      <c r="AB31" s="20"/>
+      <c r="AC31" s="20"/>
+      <c r="AD31" s="20"/>
+      <c r="AE31" s="20"/>
+      <c r="AF31" s="20"/>
+      <c r="AG31" s="20"/>
       <c r="AH31" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="AI31" s="19" t="n">
+      <c r="AI31" s="20" t="n">
         <v>0.3</v>
       </c>
     </row>
@@ -9432,47 +10045,47 @@
         <f aca="false">Populations!$C$4</f>
         <v>F 15-49</v>
       </c>
-      <c r="C32" s="19"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="19"/>
-      <c r="G32" s="19"/>
-      <c r="H32" s="19"/>
-      <c r="I32" s="19"/>
-      <c r="J32" s="19"/>
-      <c r="K32" s="19"/>
-      <c r="L32" s="19"/>
-      <c r="M32" s="19"/>
-      <c r="N32" s="19"/>
-      <c r="O32" s="19"/>
-      <c r="P32" s="19"/>
-      <c r="Q32" s="19"/>
-      <c r="R32" s="19"/>
-      <c r="S32" s="19"/>
-      <c r="T32" s="19"/>
-      <c r="U32" s="19"/>
-      <c r="V32" s="19"/>
-      <c r="W32" s="19"/>
-      <c r="X32" s="19"/>
-      <c r="Y32" s="19"/>
-      <c r="Z32" s="19"/>
-      <c r="AA32" s="19"/>
-      <c r="AB32" s="19"/>
-      <c r="AC32" s="19"/>
-      <c r="AD32" s="19"/>
-      <c r="AE32" s="19"/>
-      <c r="AF32" s="19"/>
-      <c r="AG32" s="19"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="20"/>
+      <c r="J32" s="20"/>
+      <c r="K32" s="20"/>
+      <c r="L32" s="20"/>
+      <c r="M32" s="20"/>
+      <c r="N32" s="20"/>
+      <c r="O32" s="20"/>
+      <c r="P32" s="20"/>
+      <c r="Q32" s="20"/>
+      <c r="R32" s="20"/>
+      <c r="S32" s="20"/>
+      <c r="T32" s="20"/>
+      <c r="U32" s="20"/>
+      <c r="V32" s="20"/>
+      <c r="W32" s="20"/>
+      <c r="X32" s="20"/>
+      <c r="Y32" s="20"/>
+      <c r="Z32" s="20"/>
+      <c r="AA32" s="20"/>
+      <c r="AB32" s="20"/>
+      <c r="AC32" s="20"/>
+      <c r="AD32" s="20"/>
+      <c r="AE32" s="20"/>
+      <c r="AF32" s="20"/>
+      <c r="AG32" s="20"/>
       <c r="AH32" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="AI32" s="19" t="n">
+      <c r="AI32" s="20" t="n">
         <v>0.4</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9578,41 +10191,41 @@
         <f aca="false">Populations!$C$3</f>
         <v>M 15-49</v>
       </c>
-      <c r="C38" s="19"/>
-      <c r="D38" s="19"/>
-      <c r="E38" s="19"/>
-      <c r="F38" s="19"/>
-      <c r="G38" s="19"/>
-      <c r="H38" s="19"/>
-      <c r="I38" s="19"/>
-      <c r="J38" s="19"/>
-      <c r="K38" s="19"/>
-      <c r="L38" s="19"/>
-      <c r="M38" s="19"/>
-      <c r="N38" s="19"/>
-      <c r="O38" s="19"/>
-      <c r="P38" s="19"/>
-      <c r="Q38" s="19"/>
-      <c r="R38" s="19"/>
-      <c r="S38" s="19"/>
-      <c r="T38" s="19"/>
-      <c r="U38" s="19"/>
-      <c r="V38" s="19"/>
-      <c r="W38" s="19"/>
-      <c r="X38" s="19"/>
-      <c r="Y38" s="19"/>
-      <c r="Z38" s="19"/>
-      <c r="AA38" s="19"/>
-      <c r="AB38" s="19"/>
-      <c r="AC38" s="19"/>
-      <c r="AD38" s="19"/>
-      <c r="AE38" s="19"/>
-      <c r="AF38" s="19"/>
-      <c r="AG38" s="19"/>
+      <c r="C38" s="20"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="20"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="20"/>
+      <c r="H38" s="20"/>
+      <c r="I38" s="20"/>
+      <c r="J38" s="20"/>
+      <c r="K38" s="20"/>
+      <c r="L38" s="20"/>
+      <c r="M38" s="20"/>
+      <c r="N38" s="20"/>
+      <c r="O38" s="20"/>
+      <c r="P38" s="20"/>
+      <c r="Q38" s="20"/>
+      <c r="R38" s="20"/>
+      <c r="S38" s="20"/>
+      <c r="T38" s="20"/>
+      <c r="U38" s="20"/>
+      <c r="V38" s="20"/>
+      <c r="W38" s="20"/>
+      <c r="X38" s="20"/>
+      <c r="Y38" s="20"/>
+      <c r="Z38" s="20"/>
+      <c r="AA38" s="20"/>
+      <c r="AB38" s="20"/>
+      <c r="AC38" s="20"/>
+      <c r="AD38" s="20"/>
+      <c r="AE38" s="20"/>
+      <c r="AF38" s="20"/>
+      <c r="AG38" s="20"/>
       <c r="AH38" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="AI38" s="24" t="n">
+      <c r="AI38" s="25" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9621,47 +10234,47 @@
         <f aca="false">Populations!$C$4</f>
         <v>F 15-49</v>
       </c>
-      <c r="C39" s="19"/>
-      <c r="D39" s="19"/>
-      <c r="E39" s="19"/>
-      <c r="F39" s="19"/>
-      <c r="G39" s="19"/>
-      <c r="H39" s="19"/>
-      <c r="I39" s="19"/>
-      <c r="J39" s="19"/>
-      <c r="K39" s="19"/>
-      <c r="L39" s="19"/>
-      <c r="M39" s="19"/>
-      <c r="N39" s="19"/>
-      <c r="O39" s="19"/>
-      <c r="P39" s="19"/>
-      <c r="Q39" s="19"/>
-      <c r="R39" s="19"/>
-      <c r="S39" s="19"/>
-      <c r="T39" s="19"/>
-      <c r="U39" s="19"/>
-      <c r="V39" s="19"/>
-      <c r="W39" s="19"/>
-      <c r="X39" s="19"/>
-      <c r="Y39" s="19"/>
-      <c r="Z39" s="19"/>
-      <c r="AA39" s="19"/>
-      <c r="AB39" s="19"/>
-      <c r="AC39" s="19"/>
-      <c r="AD39" s="19"/>
-      <c r="AE39" s="19"/>
-      <c r="AF39" s="19"/>
-      <c r="AG39" s="19"/>
+      <c r="C39" s="20"/>
+      <c r="D39" s="20"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="20"/>
+      <c r="G39" s="20"/>
+      <c r="H39" s="20"/>
+      <c r="I39" s="20"/>
+      <c r="J39" s="20"/>
+      <c r="K39" s="20"/>
+      <c r="L39" s="20"/>
+      <c r="M39" s="20"/>
+      <c r="N39" s="20"/>
+      <c r="O39" s="20"/>
+      <c r="P39" s="20"/>
+      <c r="Q39" s="20"/>
+      <c r="R39" s="20"/>
+      <c r="S39" s="20"/>
+      <c r="T39" s="20"/>
+      <c r="U39" s="20"/>
+      <c r="V39" s="20"/>
+      <c r="W39" s="20"/>
+      <c r="X39" s="20"/>
+      <c r="Y39" s="20"/>
+      <c r="Z39" s="20"/>
+      <c r="AA39" s="20"/>
+      <c r="AB39" s="20"/>
+      <c r="AC39" s="20"/>
+      <c r="AD39" s="20"/>
+      <c r="AE39" s="20"/>
+      <c r="AF39" s="20"/>
+      <c r="AG39" s="20"/>
       <c r="AH39" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="AI39" s="23" t="n">
+      <c r="AI39" s="24" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="3" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9767,41 +10380,41 @@
         <f aca="false">Populations!$C$3</f>
         <v>M 15-49</v>
       </c>
-      <c r="C45" s="19"/>
-      <c r="D45" s="19"/>
-      <c r="E45" s="19"/>
-      <c r="F45" s="19"/>
-      <c r="G45" s="19"/>
-      <c r="H45" s="19"/>
-      <c r="I45" s="19"/>
-      <c r="J45" s="19"/>
-      <c r="K45" s="19"/>
-      <c r="L45" s="19"/>
-      <c r="M45" s="19"/>
-      <c r="N45" s="19"/>
-      <c r="O45" s="19"/>
-      <c r="P45" s="19"/>
-      <c r="Q45" s="19"/>
-      <c r="R45" s="19"/>
-      <c r="S45" s="19"/>
-      <c r="T45" s="19"/>
-      <c r="U45" s="19"/>
-      <c r="V45" s="19"/>
-      <c r="W45" s="19"/>
-      <c r="X45" s="19"/>
-      <c r="Y45" s="19"/>
-      <c r="Z45" s="19"/>
-      <c r="AA45" s="19"/>
-      <c r="AB45" s="19"/>
-      <c r="AC45" s="19"/>
-      <c r="AD45" s="19"/>
-      <c r="AE45" s="19"/>
-      <c r="AF45" s="19"/>
-      <c r="AG45" s="19"/>
+      <c r="C45" s="20"/>
+      <c r="D45" s="20"/>
+      <c r="E45" s="20"/>
+      <c r="F45" s="20"/>
+      <c r="G45" s="20"/>
+      <c r="H45" s="20"/>
+      <c r="I45" s="20"/>
+      <c r="J45" s="20"/>
+      <c r="K45" s="20"/>
+      <c r="L45" s="20"/>
+      <c r="M45" s="20"/>
+      <c r="N45" s="20"/>
+      <c r="O45" s="20"/>
+      <c r="P45" s="20"/>
+      <c r="Q45" s="20"/>
+      <c r="R45" s="20"/>
+      <c r="S45" s="20"/>
+      <c r="T45" s="20"/>
+      <c r="U45" s="20"/>
+      <c r="V45" s="20"/>
+      <c r="W45" s="20"/>
+      <c r="X45" s="20"/>
+      <c r="Y45" s="20"/>
+      <c r="Z45" s="20"/>
+      <c r="AA45" s="20"/>
+      <c r="AB45" s="20"/>
+      <c r="AC45" s="20"/>
+      <c r="AD45" s="20"/>
+      <c r="AE45" s="20"/>
+      <c r="AF45" s="20"/>
+      <c r="AG45" s="20"/>
       <c r="AH45" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="AI45" s="23" t="n">
+      <c r="AI45" s="24" t="n">
         <v>0.1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
change reinitiation to rate not time; percentage not number
</commit_message>
<xml_diff>
--- a/tests/cascade2p.xlsx
+++ b/tests/cascade2p.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" state="visible" r:id="rId2"/>
@@ -283,7 +283,7 @@
     <t>Viral load monitoring (number/year)</t>
   </si>
   <si>
-    <t>Time to ART re-initiation (years)</t>
+    <t>Rate of ART re-initiation (%/year)</t>
   </si>
   <si>
     <t>PLHIV aware of their status (%)</t>
@@ -746,6 +746,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
+    <xf numFmtId="168" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
     <xf numFmtId="170" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
@@ -779,10 +783,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -867,15 +867,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>351000</xdr:colOff>
+      <xdr:colOff>378000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>422640</xdr:colOff>
+      <xdr:colOff>449280</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>33480</xdr:rowOff>
+      <xdr:rowOff>33120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -884,8 +884,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="351000" y="0"/>
-          <a:ext cx="25572960" cy="7120080"/>
+          <a:off x="378000" y="0"/>
+          <a:ext cx="27513360" cy="7119720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -912,15 +912,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>351000</xdr:colOff>
+      <xdr:colOff>378000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>422640</xdr:colOff>
+      <xdr:colOff>449280</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>33480</xdr:rowOff>
+      <xdr:rowOff>33120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -929,8 +929,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="351000" y="0"/>
-          <a:ext cx="25572960" cy="7120080"/>
+          <a:off x="378000" y="0"/>
+          <a:ext cx="27513360" cy="7119720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -957,15 +957,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>351000</xdr:colOff>
+      <xdr:colOff>378000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>422640</xdr:colOff>
+      <xdr:colOff>449280</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>33480</xdr:rowOff>
+      <xdr:rowOff>33120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -974,8 +974,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="351000" y="0"/>
-          <a:ext cx="25572960" cy="7120080"/>
+          <a:off x="378000" y="0"/>
+          <a:ext cx="27513360" cy="7119720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1002,15 +1002,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>351000</xdr:colOff>
+      <xdr:colOff>378000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>422640</xdr:colOff>
+      <xdr:colOff>449280</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>33480</xdr:rowOff>
+      <xdr:rowOff>33120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1019,8 +1019,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="351000" y="0"/>
-          <a:ext cx="25572960" cy="7120080"/>
+          <a:off x="378000" y="0"/>
+          <a:ext cx="27513360" cy="7119720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1047,15 +1047,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>351000</xdr:colOff>
+      <xdr:colOff>378000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>422640</xdr:colOff>
+      <xdr:colOff>449280</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>33480</xdr:rowOff>
+      <xdr:rowOff>33120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1064,8 +1064,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="351000" y="0"/>
-          <a:ext cx="25572960" cy="7120080"/>
+          <a:off x="378000" y="0"/>
+          <a:ext cx="27513360" cy="7119720"/>
         </a:xfrm>
         <a:solidFill>
           <a:srgbClr val="ffffff"/>
@@ -1094,15 +1094,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>351000</xdr:colOff>
+      <xdr:colOff>378000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>422640</xdr:colOff>
+      <xdr:colOff>449280</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>33480</xdr:rowOff>
+      <xdr:rowOff>33120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1111,8 +1111,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="351000" y="0"/>
-          <a:ext cx="25572960" cy="7310520"/>
+          <a:off x="378000" y="0"/>
+          <a:ext cx="27513360" cy="7310160"/>
         </a:xfrm>
         <a:solidFill>
           <a:srgbClr val="ffffff"/>
@@ -1141,15 +1141,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>351000</xdr:colOff>
+      <xdr:colOff>378000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>422640</xdr:colOff>
+      <xdr:colOff>449280</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>90720</xdr:rowOff>
+      <xdr:rowOff>90360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1158,8 +1158,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="351000" y="0"/>
-          <a:ext cx="25572960" cy="8434440"/>
+          <a:off x="378000" y="0"/>
+          <a:ext cx="27513360" cy="8434080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1186,15 +1186,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>351000</xdr:colOff>
+      <xdr:colOff>378000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>422640</xdr:colOff>
+      <xdr:colOff>449280</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>90720</xdr:rowOff>
+      <xdr:rowOff>90360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1203,8 +1203,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="351000" y="0"/>
-          <a:ext cx="25572960" cy="8434440"/>
+          <a:off x="378000" y="0"/>
+          <a:ext cx="27513360" cy="8434080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1231,15 +1231,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>351000</xdr:colOff>
+      <xdr:colOff>378000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>422640</xdr:colOff>
+      <xdr:colOff>449280</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>90720</xdr:rowOff>
+      <xdr:rowOff>90360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1248,8 +1248,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="351000" y="0"/>
-          <a:ext cx="25572960" cy="8434440"/>
+          <a:off x="378000" y="0"/>
+          <a:ext cx="27513360" cy="8434080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1276,15 +1276,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>351000</xdr:colOff>
+      <xdr:colOff>378000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>422640</xdr:colOff>
+      <xdr:colOff>449280</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>90720</xdr:rowOff>
+      <xdr:rowOff>90360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1293,8 +1293,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="351000" y="0"/>
-          <a:ext cx="25572960" cy="8434440"/>
+          <a:off x="378000" y="0"/>
+          <a:ext cx="27513360" cy="8434080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1321,15 +1321,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>351000</xdr:colOff>
+      <xdr:colOff>378000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>422640</xdr:colOff>
+      <xdr:colOff>449280</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>90720</xdr:rowOff>
+      <xdr:rowOff>90360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1338,8 +1338,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="351000" y="0"/>
-          <a:ext cx="25572960" cy="9767880"/>
+          <a:off x="378000" y="0"/>
+          <a:ext cx="27513360" cy="9767520"/>
         </a:xfrm>
         <a:solidFill>
           <a:srgbClr val="ffffff"/>
@@ -1368,15 +1368,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>351000</xdr:colOff>
+      <xdr:colOff>378000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>422640</xdr:colOff>
+      <xdr:colOff>449280</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>52560</xdr:rowOff>
+      <xdr:rowOff>52200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1385,8 +1385,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="351000" y="0"/>
-          <a:ext cx="25572960" cy="7805880"/>
+          <a:off x="378000" y="0"/>
+          <a:ext cx="27513360" cy="7805520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1413,15 +1413,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>351000</xdr:colOff>
+      <xdr:colOff>378000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>422640</xdr:colOff>
+      <xdr:colOff>449280</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>52560</xdr:rowOff>
+      <xdr:rowOff>52200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1430,8 +1430,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="351000" y="0"/>
-          <a:ext cx="25572960" cy="7805880"/>
+          <a:off x="378000" y="0"/>
+          <a:ext cx="27513360" cy="7805520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1458,15 +1458,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>351000</xdr:colOff>
+      <xdr:colOff>378000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>422640</xdr:colOff>
+      <xdr:colOff>449280</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>52560</xdr:rowOff>
+      <xdr:rowOff>52200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1475,8 +1475,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="351000" y="0"/>
-          <a:ext cx="25572960" cy="7805880"/>
+          <a:off x="378000" y="0"/>
+          <a:ext cx="27513360" cy="7805520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1503,15 +1503,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>351000</xdr:colOff>
+      <xdr:colOff>378000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>422640</xdr:colOff>
+      <xdr:colOff>449280</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>52560</xdr:rowOff>
+      <xdr:rowOff>52200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1520,8 +1520,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="351000" y="0"/>
-          <a:ext cx="25572960" cy="7805880"/>
+          <a:off x="378000" y="0"/>
+          <a:ext cx="27513360" cy="7805520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1548,15 +1548,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>351000</xdr:colOff>
+      <xdr:colOff>378000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>422640</xdr:colOff>
+      <xdr:colOff>449280</xdr:colOff>
       <xdr:row>55</xdr:row>
-      <xdr:rowOff>52560</xdr:rowOff>
+      <xdr:rowOff>52200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1565,8 +1565,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="351000" y="0"/>
-          <a:ext cx="25572960" cy="10091880"/>
+          <a:off x="378000" y="0"/>
+          <a:ext cx="27513360" cy="10091520"/>
         </a:xfrm>
         <a:solidFill>
           <a:srgbClr val="ffffff"/>
@@ -1595,15 +1595,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>351000</xdr:colOff>
+      <xdr:colOff>378000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>422640</xdr:colOff>
+      <xdr:colOff>449280</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>90720</xdr:rowOff>
+      <xdr:rowOff>90360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1612,8 +1612,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="351000" y="0"/>
-          <a:ext cx="25572960" cy="9863280"/>
+          <a:off x="378000" y="0"/>
+          <a:ext cx="27513360" cy="9862920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1640,15 +1640,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>351000</xdr:colOff>
+      <xdr:colOff>378000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>422640</xdr:colOff>
+      <xdr:colOff>449280</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>90720</xdr:rowOff>
+      <xdr:rowOff>90360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1657,8 +1657,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="351000" y="0"/>
-          <a:ext cx="25572960" cy="9863280"/>
+          <a:off x="378000" y="0"/>
+          <a:ext cx="27513360" cy="9862920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1685,15 +1685,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>351000</xdr:colOff>
+      <xdr:colOff>378000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>422640</xdr:colOff>
+      <xdr:colOff>449280</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>90720</xdr:rowOff>
+      <xdr:rowOff>90360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1702,8 +1702,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="351000" y="0"/>
-          <a:ext cx="25572960" cy="9863280"/>
+          <a:off x="378000" y="0"/>
+          <a:ext cx="27513360" cy="9862920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1730,15 +1730,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>351000</xdr:colOff>
+      <xdr:colOff>378000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>422640</xdr:colOff>
+      <xdr:colOff>449280</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>90720</xdr:rowOff>
+      <xdr:rowOff>90360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1747,8 +1747,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="351000" y="0"/>
-          <a:ext cx="25572960" cy="9863280"/>
+          <a:off x="378000" y="0"/>
+          <a:ext cx="27513360" cy="9862920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1775,15 +1775,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>351000</xdr:colOff>
+      <xdr:colOff>378000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>422640</xdr:colOff>
+      <xdr:colOff>449280</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>90720</xdr:rowOff>
+      <xdr:rowOff>90360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1792,8 +1792,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="351000" y="0"/>
-          <a:ext cx="25572960" cy="9863280"/>
+          <a:off x="378000" y="0"/>
+          <a:ext cx="27513360" cy="9862920"/>
         </a:xfrm>
         <a:solidFill>
           <a:srgbClr val="ffffff"/>
@@ -1830,8 +1830,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="244.15306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="19.265306122449"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="263.775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="20.7551020408163"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1888,8 +1888,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="35" min="1" style="0" width="22.5867346938776"/>
-    <col collapsed="false" hidden="false" max="1025" min="36" style="0" width="19.265306122449"/>
+    <col collapsed="false" hidden="false" max="35" min="1" style="0" width="24.3061224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="36" style="0" width="20.7551020408163"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2189,41 +2189,41 @@
         <f aca="false">Populations!$C$3</f>
         <v>M 15-49</v>
       </c>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="20"/>
-      <c r="M10" s="20"/>
-      <c r="N10" s="20"/>
-      <c r="O10" s="20"/>
-      <c r="P10" s="20"/>
-      <c r="Q10" s="20"/>
-      <c r="R10" s="20"/>
-      <c r="S10" s="20"/>
-      <c r="T10" s="20"/>
-      <c r="U10" s="20"/>
-      <c r="V10" s="20"/>
-      <c r="W10" s="20"/>
-      <c r="X10" s="20"/>
-      <c r="Y10" s="20"/>
-      <c r="Z10" s="20"/>
-      <c r="AA10" s="20"/>
-      <c r="AB10" s="20"/>
-      <c r="AC10" s="20"/>
-      <c r="AD10" s="20"/>
-      <c r="AE10" s="20"/>
-      <c r="AF10" s="20"/>
-      <c r="AG10" s="20"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="21"/>
+      <c r="M10" s="21"/>
+      <c r="N10" s="21"/>
+      <c r="O10" s="21"/>
+      <c r="P10" s="21"/>
+      <c r="Q10" s="21"/>
+      <c r="R10" s="21"/>
+      <c r="S10" s="21"/>
+      <c r="T10" s="21"/>
+      <c r="U10" s="21"/>
+      <c r="V10" s="21"/>
+      <c r="W10" s="21"/>
+      <c r="X10" s="21"/>
+      <c r="Y10" s="21"/>
+      <c r="Z10" s="21"/>
+      <c r="AA10" s="21"/>
+      <c r="AB10" s="21"/>
+      <c r="AC10" s="21"/>
+      <c r="AD10" s="21"/>
+      <c r="AE10" s="21"/>
+      <c r="AF10" s="21"/>
+      <c r="AG10" s="21"/>
       <c r="AH10" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="AI10" s="20" t="n">
+      <c r="AI10" s="21" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2232,41 +2232,41 @@
         <f aca="false">Populations!$C$4</f>
         <v>F 15-49</v>
       </c>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="20"/>
-      <c r="M11" s="20"/>
-      <c r="N11" s="20"/>
-      <c r="O11" s="20"/>
-      <c r="P11" s="20"/>
-      <c r="Q11" s="20"/>
-      <c r="R11" s="20"/>
-      <c r="S11" s="20"/>
-      <c r="T11" s="20"/>
-      <c r="U11" s="20"/>
-      <c r="V11" s="20"/>
-      <c r="W11" s="20"/>
-      <c r="X11" s="20"/>
-      <c r="Y11" s="20"/>
-      <c r="Z11" s="20"/>
-      <c r="AA11" s="20"/>
-      <c r="AB11" s="20"/>
-      <c r="AC11" s="20"/>
-      <c r="AD11" s="20"/>
-      <c r="AE11" s="20"/>
-      <c r="AF11" s="20"/>
-      <c r="AG11" s="20"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="21"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="21"/>
+      <c r="L11" s="21"/>
+      <c r="M11" s="21"/>
+      <c r="N11" s="21"/>
+      <c r="O11" s="21"/>
+      <c r="P11" s="21"/>
+      <c r="Q11" s="21"/>
+      <c r="R11" s="21"/>
+      <c r="S11" s="21"/>
+      <c r="T11" s="21"/>
+      <c r="U11" s="21"/>
+      <c r="V11" s="21"/>
+      <c r="W11" s="21"/>
+      <c r="X11" s="21"/>
+      <c r="Y11" s="21"/>
+      <c r="Z11" s="21"/>
+      <c r="AA11" s="21"/>
+      <c r="AB11" s="21"/>
+      <c r="AC11" s="21"/>
+      <c r="AD11" s="21"/>
+      <c r="AE11" s="21"/>
+      <c r="AF11" s="21"/>
+      <c r="AG11" s="21"/>
       <c r="AH11" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="AI11" s="20" t="n">
+      <c r="AI11" s="21" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2439,10 +2439,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="22.5867346938776"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="33.6020408163265"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="22.5867346938776"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="19.265306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="24.3061224489796"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="36.2397959183673"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="24.3061224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="20.7551020408163"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2682,9 +2682,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.265306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="110.780612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="19.265306122449"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.7551020408163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="119.612244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="20.7551020408163"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2704,100 +2704,100 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="C3" s="27" t="n">
+      <c r="C3" s="28" t="n">
         <v>0.0004</v>
       </c>
-      <c r="D3" s="27" t="n">
+      <c r="D3" s="28" t="n">
         <v>0.0001</v>
       </c>
-      <c r="E3" s="27" t="n">
+      <c r="E3" s="28" t="n">
         <v>0.0014</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="C4" s="27" t="n">
+      <c r="C4" s="28" t="n">
         <v>0.0008</v>
       </c>
-      <c r="D4" s="27" t="n">
+      <c r="D4" s="28" t="n">
         <v>0.0006</v>
       </c>
-      <c r="E4" s="27" t="n">
+      <c r="E4" s="28" t="n">
         <v>0.0011</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="C5" s="27" t="n">
+      <c r="C5" s="28" t="n">
         <v>0.0138</v>
       </c>
-      <c r="D5" s="27" t="n">
+      <c r="D5" s="28" t="n">
         <v>0.0102</v>
       </c>
-      <c r="E5" s="27" t="n">
+      <c r="E5" s="28" t="n">
         <v>0.0186</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="C6" s="27" t="n">
+      <c r="C6" s="28" t="n">
         <v>0.0011</v>
       </c>
-      <c r="D6" s="27" t="n">
+      <c r="D6" s="28" t="n">
         <v>0.0004</v>
       </c>
-      <c r="E6" s="27" t="n">
+      <c r="E6" s="28" t="n">
         <v>0.0028</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="C7" s="27" t="n">
+      <c r="C7" s="28" t="n">
         <v>0.008</v>
       </c>
-      <c r="D7" s="27" t="n">
+      <c r="D7" s="28" t="n">
         <v>0.0063</v>
       </c>
-      <c r="E7" s="27" t="n">
+      <c r="E7" s="28" t="n">
         <v>0.024</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="C8" s="27" t="n">
+      <c r="C8" s="28" t="n">
         <v>0.367</v>
       </c>
-      <c r="D8" s="27" t="n">
+      <c r="D8" s="28" t="n">
         <v>0.294</v>
       </c>
-      <c r="E8" s="27" t="n">
+      <c r="E8" s="28" t="n">
         <v>0.44</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="C9" s="27" t="n">
+      <c r="C9" s="28" t="n">
         <v>0.205</v>
       </c>
-      <c r="D9" s="27" t="n">
+      <c r="D9" s="28" t="n">
         <v>0.14</v>
       </c>
-      <c r="E9" s="27" t="n">
+      <c r="E9" s="28" t="n">
         <v>0.27</v>
       </c>
     </row>
@@ -2827,86 +2827,86 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="26" t="s">
+      <c r="B15" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="C15" s="28" t="n">
+      <c r="C15" s="19" t="n">
         <v>26.03</v>
       </c>
-      <c r="D15" s="28" t="n">
+      <c r="D15" s="19" t="n">
         <v>2</v>
       </c>
-      <c r="E15" s="28" t="n">
+      <c r="E15" s="19" t="n">
         <v>48.02</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B16" s="26" t="s">
+      <c r="B16" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="C16" s="28" t="n">
+      <c r="C16" s="19" t="n">
         <v>1</v>
       </c>
-      <c r="D16" s="28" t="n">
+      <c r="D16" s="19" t="n">
         <v>1</v>
       </c>
-      <c r="E16" s="28" t="n">
+      <c r="E16" s="19" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B17" s="26" t="s">
+      <c r="B17" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="C17" s="28" t="n">
+      <c r="C17" s="19" t="n">
         <v>1</v>
       </c>
-      <c r="D17" s="28" t="n">
+      <c r="D17" s="19" t="n">
         <v>1</v>
       </c>
-      <c r="E17" s="28" t="n">
+      <c r="E17" s="19" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B18" s="26" t="s">
+      <c r="B18" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="C18" s="28" t="n">
+      <c r="C18" s="19" t="n">
         <v>1</v>
       </c>
-      <c r="D18" s="28" t="n">
+      <c r="D18" s="19" t="n">
         <v>1</v>
       </c>
-      <c r="E18" s="28" t="n">
+      <c r="E18" s="19" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B19" s="26" t="s">
+      <c r="B19" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="C19" s="28" t="n">
+      <c r="C19" s="19" t="n">
         <v>3.49</v>
       </c>
-      <c r="D19" s="28" t="n">
+      <c r="D19" s="19" t="n">
         <v>1.76</v>
       </c>
-      <c r="E19" s="28" t="n">
+      <c r="E19" s="19" t="n">
         <v>6.92</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B20" s="26" t="s">
+      <c r="B20" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="C20" s="28" t="n">
+      <c r="C20" s="19" t="n">
         <v>7.17</v>
       </c>
-      <c r="D20" s="28" t="n">
+      <c r="D20" s="19" t="n">
         <v>3.9</v>
       </c>
-      <c r="E20" s="28" t="n">
+      <c r="E20" s="19" t="n">
         <v>12.08</v>
       </c>
     </row>
@@ -2936,7 +2936,7 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B26" s="26" t="s">
+      <c r="B26" s="27" t="s">
         <v>86</v>
       </c>
       <c r="C26" s="18" t="n">
@@ -2950,7 +2950,7 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B27" s="26" t="s">
+      <c r="B27" s="27" t="s">
         <v>81</v>
       </c>
       <c r="C27" s="18" t="n">
@@ -2964,7 +2964,7 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B28" s="26" t="s">
+      <c r="B28" s="27" t="s">
         <v>87</v>
       </c>
       <c r="C28" s="18" t="n">
@@ -2978,7 +2978,7 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B29" s="26" t="s">
+      <c r="B29" s="27" t="s">
         <v>88</v>
       </c>
       <c r="C29" s="18" t="n">
@@ -2992,7 +2992,7 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B30" s="26" t="s">
+      <c r="B30" s="27" t="s">
         <v>89</v>
       </c>
       <c r="C30" s="18" t="n">
@@ -3031,7 +3031,7 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B36" s="26" t="s">
+      <c r="B36" s="27" t="s">
         <v>91</v>
       </c>
       <c r="C36" s="18" t="n">
@@ -3045,7 +3045,7 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B37" s="26" t="s">
+      <c r="B37" s="27" t="s">
         <v>92</v>
       </c>
       <c r="C37" s="18" t="n">
@@ -3059,7 +3059,7 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B38" s="26" t="s">
+      <c r="B38" s="27" t="s">
         <v>93</v>
       </c>
       <c r="C38" s="18" t="n">
@@ -3073,7 +3073,7 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B39" s="26" t="s">
+      <c r="B39" s="27" t="s">
         <v>94</v>
       </c>
       <c r="C39" s="18" t="n">
@@ -3112,114 +3112,114 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B45" s="26" t="s">
+      <c r="B45" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="C45" s="27" t="n">
+      <c r="C45" s="28" t="n">
         <v>0.0036</v>
       </c>
-      <c r="D45" s="27" t="n">
+      <c r="D45" s="28" t="n">
         <v>0.0029</v>
       </c>
-      <c r="E45" s="27" t="n">
+      <c r="E45" s="28" t="n">
         <v>0.0044</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B46" s="26" t="s">
+      <c r="B46" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="C46" s="27" t="n">
+      <c r="C46" s="28" t="n">
         <v>0.0036</v>
       </c>
-      <c r="D46" s="27" t="n">
+      <c r="D46" s="28" t="n">
         <v>0.0029</v>
       </c>
-      <c r="E46" s="27" t="n">
+      <c r="E46" s="28" t="n">
         <v>0.0044</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B47" s="26" t="s">
+      <c r="B47" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="C47" s="27" t="n">
+      <c r="C47" s="28" t="n">
         <v>0.0058</v>
       </c>
-      <c r="D47" s="27" t="n">
+      <c r="D47" s="28" t="n">
         <v>0.0048</v>
       </c>
-      <c r="E47" s="27" t="n">
+      <c r="E47" s="28" t="n">
         <v>0.0071</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B48" s="26" t="s">
+      <c r="B48" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="C48" s="27" t="n">
+      <c r="C48" s="28" t="n">
         <v>0.0088</v>
       </c>
-      <c r="D48" s="27" t="n">
+      <c r="D48" s="28" t="n">
         <v>0.075</v>
       </c>
-      <c r="E48" s="27" t="n">
+      <c r="E48" s="28" t="n">
         <v>0.0101</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B49" s="26" t="s">
+      <c r="B49" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="C49" s="27" t="n">
+      <c r="C49" s="28" t="n">
         <v>0.059</v>
       </c>
-      <c r="D49" s="27" t="n">
+      <c r="D49" s="28" t="n">
         <v>0.054</v>
       </c>
-      <c r="E49" s="27" t="n">
+      <c r="E49" s="28" t="n">
         <v>0.079</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B50" s="26" t="s">
+      <c r="B50" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="C50" s="27" t="n">
+      <c r="C50" s="28" t="n">
         <v>0.323</v>
       </c>
-      <c r="D50" s="27" t="n">
+      <c r="D50" s="28" t="n">
         <v>0.296</v>
       </c>
-      <c r="E50" s="27" t="n">
+      <c r="E50" s="28" t="n">
         <v>0.432</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B51" s="26" t="s">
+      <c r="B51" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="C51" s="27" t="n">
+      <c r="C51" s="28" t="n">
         <v>0.23</v>
       </c>
-      <c r="D51" s="27" t="n">
+      <c r="D51" s="28" t="n">
         <v>0.15</v>
       </c>
-      <c r="E51" s="27" t="n">
+      <c r="E51" s="28" t="n">
         <v>0.3</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B52" s="26" t="s">
+      <c r="B52" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="C52" s="27" t="n">
+      <c r="C52" s="28" t="n">
         <v>2.17</v>
       </c>
-      <c r="D52" s="27" t="n">
+      <c r="D52" s="28" t="n">
         <v>1.27</v>
       </c>
-      <c r="E52" s="27" t="n">
+      <c r="E52" s="28" t="n">
         <v>3.71</v>
       </c>
     </row>
@@ -3249,7 +3249,7 @@
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B58" s="26" t="s">
+      <c r="B58" s="27" t="s">
         <v>100</v>
       </c>
       <c r="C58" s="18" t="n">
@@ -3266,7 +3266,7 @@
       <c r="I58" s="29"/>
     </row>
     <row r="59" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B59" s="26" t="s">
+      <c r="B59" s="27" t="s">
         <v>101</v>
       </c>
       <c r="C59" s="18" t="n">
@@ -3283,7 +3283,7 @@
       <c r="I59" s="29"/>
     </row>
     <row r="60" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B60" s="26" t="s">
+      <c r="B60" s="27" t="s">
         <v>102</v>
       </c>
       <c r="C60" s="18" t="n">
@@ -3300,7 +3300,7 @@
       <c r="I60" s="29"/>
     </row>
     <row r="61" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B61" s="26" t="s">
+      <c r="B61" s="27" t="s">
         <v>103</v>
       </c>
       <c r="C61" s="18" t="n">
@@ -3317,7 +3317,7 @@
       <c r="I61" s="29"/>
     </row>
     <row r="62" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B62" s="26" t="s">
+      <c r="B62" s="27" t="s">
         <v>104</v>
       </c>
       <c r="C62" s="18" t="n">
@@ -3334,7 +3334,7 @@
       <c r="I62" s="29"/>
     </row>
     <row r="63" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B63" s="26" t="s">
+      <c r="B63" s="27" t="s">
         <v>105</v>
       </c>
       <c r="C63" s="18" t="n">
@@ -3351,7 +3351,7 @@
       <c r="I63" s="29"/>
     </row>
     <row r="64" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B64" s="26" t="s">
+      <c r="B64" s="27" t="s">
         <v>106</v>
       </c>
       <c r="C64" s="18" t="n">
@@ -3368,7 +3368,7 @@
       <c r="I64" s="29"/>
     </row>
     <row r="65" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B65" s="26" t="s">
+      <c r="B65" s="27" t="s">
         <v>107</v>
       </c>
       <c r="C65" s="18" t="n">
@@ -3385,7 +3385,7 @@
       <c r="I65" s="29"/>
     </row>
     <row r="66" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B66" s="26" t="s">
+      <c r="B66" s="27" t="s">
         <v>108</v>
       </c>
       <c r="C66" s="18" t="n">
@@ -3399,7 +3399,7 @@
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B67" s="26" t="s">
+      <c r="B67" s="27" t="s">
         <v>109</v>
       </c>
       <c r="C67" s="18" t="n">
@@ -3432,100 +3432,100 @@
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B73" s="26" t="s">
+      <c r="B73" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="C73" s="28" t="n">
+      <c r="C73" s="19" t="n">
         <v>0.146</v>
       </c>
-      <c r="D73" s="28" t="n">
+      <c r="D73" s="19" t="n">
         <v>0.096</v>
       </c>
-      <c r="E73" s="28" t="n">
+      <c r="E73" s="19" t="n">
         <v>0.205</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B74" s="26" t="s">
+      <c r="B74" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="C74" s="28" t="n">
+      <c r="C74" s="19" t="n">
         <v>0.008</v>
       </c>
-      <c r="D74" s="28" t="n">
+      <c r="D74" s="19" t="n">
         <v>0.005</v>
       </c>
-      <c r="E74" s="28" t="n">
+      <c r="E74" s="19" t="n">
         <v>0.011</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B75" s="26" t="s">
+      <c r="B75" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="C75" s="28" t="n">
+      <c r="C75" s="19" t="n">
         <v>0.02</v>
       </c>
-      <c r="D75" s="28" t="n">
+      <c r="D75" s="19" t="n">
         <v>0.013</v>
       </c>
-      <c r="E75" s="28" t="n">
+      <c r="E75" s="19" t="n">
         <v>0.029</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B76" s="26" t="s">
+      <c r="B76" s="27" t="s">
         <v>114</v>
       </c>
-      <c r="C76" s="28" t="n">
+      <c r="C76" s="19" t="n">
         <v>0.07</v>
       </c>
-      <c r="D76" s="28" t="n">
+      <c r="D76" s="19" t="n">
         <v>0.048</v>
       </c>
-      <c r="E76" s="28" t="n">
+      <c r="E76" s="19" t="n">
         <v>0.094</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B77" s="26" t="s">
+      <c r="B77" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="C77" s="28" t="n">
+      <c r="C77" s="19" t="n">
         <v>0.265</v>
       </c>
-      <c r="D77" s="28" t="n">
+      <c r="D77" s="19" t="n">
         <v>0.114</v>
       </c>
-      <c r="E77" s="28" t="n">
+      <c r="E77" s="19" t="n">
         <v>0.474</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B78" s="26" t="s">
+      <c r="B78" s="27" t="s">
         <v>116</v>
       </c>
-      <c r="C78" s="28" t="n">
+      <c r="C78" s="19" t="n">
         <v>0.547</v>
       </c>
-      <c r="D78" s="28" t="n">
+      <c r="D78" s="19" t="n">
         <v>0.382</v>
       </c>
-      <c r="E78" s="28" t="n">
+      <c r="E78" s="19" t="n">
         <v>0.715</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B79" s="26" t="s">
+      <c r="B79" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="C79" s="28" t="n">
+      <c r="C79" s="19" t="n">
         <v>0.053</v>
       </c>
-      <c r="D79" s="28" t="n">
+      <c r="D79" s="19" t="n">
         <v>0.034</v>
       </c>
-      <c r="E79" s="28" t="n">
+      <c r="E79" s="19" t="n">
         <v>0.079</v>
       </c>
     </row>
@@ -3553,12 +3553,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="22.5867346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.9744897959184"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="110.780612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="22.5867346938776"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="33.6020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="19.265306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="24.3061224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="45.3010204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="119.612244897959"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="24.3061224489796"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.2397959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="20.7551020408163"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3677,8 +3677,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="36" min="1" style="0" width="22.5867346938776"/>
-    <col collapsed="false" hidden="false" max="1025" min="37" style="0" width="19.265306122449"/>
+    <col collapsed="false" hidden="false" max="36" min="1" style="0" width="24.3061224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="37" style="0" width="20.7551020408163"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4089,8 +4089,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="36" min="1" style="0" width="22.5867346938776"/>
-    <col collapsed="false" hidden="false" max="1025" min="37" style="0" width="19.265306122449"/>
+    <col collapsed="false" hidden="false" max="36" min="1" style="0" width="24.3061224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="37" style="0" width="20.7551020408163"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4497,8 +4497,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="35" min="1" style="0" width="22.5867346938776"/>
-    <col collapsed="false" hidden="false" max="1025" min="36" style="0" width="19.265306122449"/>
+    <col collapsed="false" hidden="false" max="35" min="1" style="0" width="24.3061224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="36" style="0" width="20.7551020408163"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5098,8 +5098,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="35" min="1" style="0" width="22.5867346938776"/>
-    <col collapsed="false" hidden="false" max="1025" min="36" style="0" width="19.265306122449"/>
+    <col collapsed="false" hidden="false" max="35" min="1" style="0" width="24.3061224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="36" style="0" width="20.7551020408163"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6121,13 +6121,13 @@
   </sheetPr>
   <dimension ref="A1:AI68"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AI19" activeCellId="0" sqref="AI19"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AF40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AI55" activeCellId="0" sqref="AI55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="19.265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="20.7551020408163"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7292,41 +7292,41 @@
       <c r="B43" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="C43" s="18"/>
-      <c r="D43" s="18"/>
-      <c r="E43" s="18"/>
-      <c r="F43" s="18"/>
-      <c r="G43" s="18"/>
-      <c r="H43" s="18"/>
-      <c r="I43" s="18"/>
-      <c r="J43" s="18"/>
-      <c r="K43" s="18"/>
-      <c r="L43" s="18"/>
-      <c r="M43" s="18"/>
-      <c r="N43" s="18"/>
-      <c r="O43" s="18"/>
-      <c r="P43" s="18"/>
-      <c r="Q43" s="18"/>
-      <c r="R43" s="18"/>
-      <c r="S43" s="18"/>
-      <c r="T43" s="18"/>
-      <c r="U43" s="18"/>
-      <c r="V43" s="18"/>
-      <c r="W43" s="18"/>
-      <c r="X43" s="18"/>
-      <c r="Y43" s="18"/>
-      <c r="Z43" s="18"/>
-      <c r="AA43" s="18"/>
-      <c r="AB43" s="18"/>
-      <c r="AC43" s="18"/>
-      <c r="AD43" s="18"/>
-      <c r="AE43" s="18"/>
-      <c r="AF43" s="18"/>
-      <c r="AG43" s="18"/>
+      <c r="C43" s="19"/>
+      <c r="D43" s="19"/>
+      <c r="E43" s="19"/>
+      <c r="F43" s="19"/>
+      <c r="G43" s="19"/>
+      <c r="H43" s="19"/>
+      <c r="I43" s="19"/>
+      <c r="J43" s="19"/>
+      <c r="K43" s="19"/>
+      <c r="L43" s="19"/>
+      <c r="M43" s="19"/>
+      <c r="N43" s="19"/>
+      <c r="O43" s="19"/>
+      <c r="P43" s="19"/>
+      <c r="Q43" s="19"/>
+      <c r="R43" s="19"/>
+      <c r="S43" s="19"/>
+      <c r="T43" s="19"/>
+      <c r="U43" s="19"/>
+      <c r="V43" s="19"/>
+      <c r="W43" s="19"/>
+      <c r="X43" s="19"/>
+      <c r="Y43" s="19"/>
+      <c r="Z43" s="19"/>
+      <c r="AA43" s="19"/>
+      <c r="AB43" s="19"/>
+      <c r="AC43" s="19"/>
+      <c r="AD43" s="19"/>
+      <c r="AE43" s="19"/>
+      <c r="AF43" s="19"/>
+      <c r="AG43" s="19"/>
       <c r="AH43" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="AI43" s="19" t="n">
+      <c r="AI43" s="20" t="n">
         <v>1</v>
       </c>
     </row>
@@ -7474,8 +7474,8 @@
       <c r="AH49" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="AI49" s="19" t="n">
-        <v>1</v>
+      <c r="AI49" s="18" t="n">
+        <v>0.95</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -7955,8 +7955,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="35" min="1" style="0" width="22.5867346938776"/>
-    <col collapsed="false" hidden="false" max="1025" min="36" style="0" width="19.265306122449"/>
+    <col collapsed="false" hidden="false" max="35" min="1" style="0" width="24.3061224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="36" style="0" width="20.7551020408163"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8067,86 +8067,86 @@
         <f aca="false">Populations!$C$3</f>
         <v>M 15-49</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="20" t="n">
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21" t="n">
         <v>0.0645</v>
       </c>
-      <c r="N3" s="20"/>
-      <c r="O3" s="20"/>
-      <c r="P3" s="20"/>
-      <c r="Q3" s="20"/>
-      <c r="R3" s="20"/>
-      <c r="S3" s="20"/>
-      <c r="T3" s="20"/>
-      <c r="U3" s="20"/>
-      <c r="V3" s="20"/>
-      <c r="W3" s="20"/>
-      <c r="X3" s="20"/>
-      <c r="Y3" s="20"/>
-      <c r="Z3" s="20"/>
-      <c r="AA3" s="20"/>
-      <c r="AB3" s="20"/>
-      <c r="AC3" s="20"/>
-      <c r="AD3" s="20"/>
-      <c r="AE3" s="20"/>
-      <c r="AF3" s="20"/>
-      <c r="AG3" s="20"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
+      <c r="Q3" s="21"/>
+      <c r="R3" s="21"/>
+      <c r="S3" s="21"/>
+      <c r="T3" s="21"/>
+      <c r="U3" s="21"/>
+      <c r="V3" s="21"/>
+      <c r="W3" s="21"/>
+      <c r="X3" s="21"/>
+      <c r="Y3" s="21"/>
+      <c r="Z3" s="21"/>
+      <c r="AA3" s="21"/>
+      <c r="AB3" s="21"/>
+      <c r="AC3" s="21"/>
+      <c r="AD3" s="21"/>
+      <c r="AE3" s="21"/>
+      <c r="AF3" s="21"/>
+      <c r="AG3" s="21"/>
       <c r="AH3" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="AI3" s="20"/>
+      <c r="AI3" s="21"/>
     </row>
     <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="6" t="str">
         <f aca="false">Populations!$C$4</f>
         <v>F 15-49</v>
       </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="20"/>
-      <c r="M4" s="20" t="n">
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="21" t="n">
         <v>0.0645</v>
       </c>
-      <c r="N4" s="20"/>
-      <c r="O4" s="20"/>
-      <c r="P4" s="20"/>
-      <c r="Q4" s="20"/>
-      <c r="R4" s="20"/>
-      <c r="S4" s="20"/>
-      <c r="T4" s="20"/>
-      <c r="U4" s="20"/>
-      <c r="V4" s="20"/>
-      <c r="W4" s="20"/>
-      <c r="X4" s="20"/>
-      <c r="Y4" s="20"/>
-      <c r="Z4" s="20"/>
-      <c r="AA4" s="20"/>
-      <c r="AB4" s="20"/>
-      <c r="AC4" s="20"/>
-      <c r="AD4" s="20"/>
-      <c r="AE4" s="20"/>
-      <c r="AF4" s="20"/>
-      <c r="AG4" s="20"/>
+      <c r="N4" s="21"/>
+      <c r="O4" s="21"/>
+      <c r="P4" s="21"/>
+      <c r="Q4" s="21"/>
+      <c r="R4" s="21"/>
+      <c r="S4" s="21"/>
+      <c r="T4" s="21"/>
+      <c r="U4" s="21"/>
+      <c r="V4" s="21"/>
+      <c r="W4" s="21"/>
+      <c r="X4" s="21"/>
+      <c r="Y4" s="21"/>
+      <c r="Z4" s="21"/>
+      <c r="AA4" s="21"/>
+      <c r="AB4" s="21"/>
+      <c r="AC4" s="21"/>
+      <c r="AD4" s="21"/>
+      <c r="AE4" s="21"/>
+      <c r="AF4" s="21"/>
+      <c r="AG4" s="21"/>
       <c r="AH4" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="AI4" s="20"/>
+      <c r="AI4" s="21"/>
     </row>
     <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
@@ -8289,7 +8289,7 @@
       <c r="AH10" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="AI10" s="21" t="n">
+      <c r="AI10" s="22" t="n">
         <v>0.65</v>
       </c>
     </row>
@@ -8556,86 +8556,86 @@
         <f aca="false">Populations!$C$3</f>
         <v>M 15-49</v>
       </c>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="20"/>
-      <c r="K22" s="20"/>
-      <c r="L22" s="20"/>
-      <c r="M22" s="20"/>
-      <c r="N22" s="20"/>
-      <c r="O22" s="20"/>
-      <c r="P22" s="20"/>
-      <c r="Q22" s="20" t="n">
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="21"/>
+      <c r="J22" s="21"/>
+      <c r="K22" s="21"/>
+      <c r="L22" s="21"/>
+      <c r="M22" s="21"/>
+      <c r="N22" s="21"/>
+      <c r="O22" s="21"/>
+      <c r="P22" s="21"/>
+      <c r="Q22" s="21" t="n">
         <v>0</v>
       </c>
-      <c r="R22" s="20"/>
-      <c r="S22" s="20"/>
-      <c r="T22" s="20"/>
-      <c r="U22" s="20"/>
-      <c r="V22" s="20"/>
-      <c r="W22" s="20"/>
-      <c r="X22" s="20"/>
-      <c r="Y22" s="20"/>
-      <c r="Z22" s="20"/>
-      <c r="AA22" s="20"/>
-      <c r="AB22" s="20"/>
-      <c r="AC22" s="20"/>
-      <c r="AD22" s="20"/>
-      <c r="AE22" s="20"/>
-      <c r="AF22" s="20"/>
-      <c r="AG22" s="20"/>
+      <c r="R22" s="21"/>
+      <c r="S22" s="21"/>
+      <c r="T22" s="21"/>
+      <c r="U22" s="21"/>
+      <c r="V22" s="21"/>
+      <c r="W22" s="21"/>
+      <c r="X22" s="21"/>
+      <c r="Y22" s="21"/>
+      <c r="Z22" s="21"/>
+      <c r="AA22" s="21"/>
+      <c r="AB22" s="21"/>
+      <c r="AC22" s="21"/>
+      <c r="AD22" s="21"/>
+      <c r="AE22" s="21"/>
+      <c r="AF22" s="21"/>
+      <c r="AG22" s="21"/>
       <c r="AH22" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="AI22" s="20"/>
+      <c r="AI22" s="21"/>
     </row>
     <row r="23" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B23" s="6" t="str">
         <f aca="false">Populations!$C$4</f>
         <v>F 15-49</v>
       </c>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="20"/>
-      <c r="K23" s="20"/>
-      <c r="L23" s="20"/>
-      <c r="M23" s="20"/>
-      <c r="N23" s="20"/>
-      <c r="O23" s="20"/>
-      <c r="P23" s="20"/>
-      <c r="Q23" s="20" t="n">
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="21"/>
+      <c r="J23" s="21"/>
+      <c r="K23" s="21"/>
+      <c r="L23" s="21"/>
+      <c r="M23" s="21"/>
+      <c r="N23" s="21"/>
+      <c r="O23" s="21"/>
+      <c r="P23" s="21"/>
+      <c r="Q23" s="21" t="n">
         <v>0</v>
       </c>
-      <c r="R23" s="20"/>
-      <c r="S23" s="20"/>
-      <c r="T23" s="20"/>
-      <c r="U23" s="20"/>
-      <c r="V23" s="20"/>
-      <c r="W23" s="20"/>
-      <c r="X23" s="20"/>
-      <c r="Y23" s="20"/>
-      <c r="Z23" s="20"/>
-      <c r="AA23" s="20"/>
-      <c r="AB23" s="20"/>
-      <c r="AC23" s="20"/>
-      <c r="AD23" s="20"/>
-      <c r="AE23" s="20"/>
-      <c r="AF23" s="20"/>
-      <c r="AG23" s="20"/>
+      <c r="R23" s="21"/>
+      <c r="S23" s="21"/>
+      <c r="T23" s="21"/>
+      <c r="U23" s="21"/>
+      <c r="V23" s="21"/>
+      <c r="W23" s="21"/>
+      <c r="X23" s="21"/>
+      <c r="Y23" s="21"/>
+      <c r="Z23" s="21"/>
+      <c r="AA23" s="21"/>
+      <c r="AB23" s="21"/>
+      <c r="AC23" s="21"/>
+      <c r="AD23" s="21"/>
+      <c r="AE23" s="21"/>
+      <c r="AF23" s="21"/>
+      <c r="AG23" s="21"/>
       <c r="AH23" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="AI23" s="20"/>
+      <c r="AI23" s="21"/>
     </row>
     <row r="27" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
@@ -9067,41 +9067,41 @@
       <c r="B41" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C41" s="20"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="20"/>
-      <c r="F41" s="20"/>
-      <c r="G41" s="20"/>
-      <c r="H41" s="20"/>
-      <c r="I41" s="20"/>
-      <c r="J41" s="20"/>
-      <c r="K41" s="20"/>
-      <c r="L41" s="20"/>
-      <c r="M41" s="20"/>
-      <c r="N41" s="20"/>
-      <c r="O41" s="20"/>
-      <c r="P41" s="20"/>
-      <c r="Q41" s="20"/>
-      <c r="R41" s="20"/>
-      <c r="S41" s="20"/>
-      <c r="T41" s="20"/>
-      <c r="U41" s="20"/>
-      <c r="V41" s="20"/>
-      <c r="W41" s="20"/>
-      <c r="X41" s="20"/>
-      <c r="Y41" s="20"/>
-      <c r="Z41" s="20"/>
-      <c r="AA41" s="20"/>
-      <c r="AB41" s="20"/>
-      <c r="AC41" s="20"/>
-      <c r="AD41" s="20"/>
-      <c r="AE41" s="20"/>
-      <c r="AF41" s="20"/>
-      <c r="AG41" s="20"/>
+      <c r="C41" s="21"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="21"/>
+      <c r="F41" s="21"/>
+      <c r="G41" s="21"/>
+      <c r="H41" s="21"/>
+      <c r="I41" s="21"/>
+      <c r="J41" s="21"/>
+      <c r="K41" s="21"/>
+      <c r="L41" s="21"/>
+      <c r="M41" s="21"/>
+      <c r="N41" s="21"/>
+      <c r="O41" s="21"/>
+      <c r="P41" s="21"/>
+      <c r="Q41" s="21"/>
+      <c r="R41" s="21"/>
+      <c r="S41" s="21"/>
+      <c r="T41" s="21"/>
+      <c r="U41" s="21"/>
+      <c r="V41" s="21"/>
+      <c r="W41" s="21"/>
+      <c r="X41" s="21"/>
+      <c r="Y41" s="21"/>
+      <c r="Z41" s="21"/>
+      <c r="AA41" s="21"/>
+      <c r="AB41" s="21"/>
+      <c r="AC41" s="21"/>
+      <c r="AD41" s="21"/>
+      <c r="AE41" s="21"/>
+      <c r="AF41" s="21"/>
+      <c r="AG41" s="21"/>
       <c r="AH41" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="AI41" s="22" t="n">
+      <c r="AI41" s="23" t="n">
         <f aca="false">14/100*87/100</f>
         <v>0.1218</v>
       </c>
@@ -9132,8 +9132,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="35" min="1" style="0" width="22.5867346938776"/>
-    <col collapsed="false" hidden="false" max="1025" min="36" style="0" width="19.265306122449"/>
+    <col collapsed="false" hidden="false" max="35" min="1" style="0" width="24.3061224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="36" style="0" width="20.7551020408163"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9278,7 +9278,7 @@
       <c r="AH3" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="AI3" s="23" t="n">
+      <c r="AI3" s="24" t="n">
         <v>100</v>
       </c>
     </row>
@@ -9321,7 +9321,7 @@
       <c r="AH4" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="AI4" s="23" t="n">
+      <c r="AI4" s="24" t="n">
         <v>100</v>
       </c>
     </row>
@@ -9467,7 +9467,7 @@
       <c r="AH10" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="AI10" s="23" t="n">
+      <c r="AI10" s="24" t="n">
         <f aca="false">0.2*3*20</f>
         <v>12</v>
       </c>
@@ -9511,7 +9511,7 @@
       <c r="AH11" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="AI11" s="23" t="n">
+      <c r="AI11" s="24" t="n">
         <f aca="false">0.1*3*20</f>
         <v>6</v>
       </c>
@@ -9813,41 +9813,41 @@
         <f aca="false">Populations!$C$3</f>
         <v>M 15-49</v>
       </c>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
-      <c r="I24" s="20"/>
-      <c r="J24" s="20"/>
-      <c r="K24" s="20"/>
-      <c r="L24" s="20"/>
-      <c r="M24" s="20"/>
-      <c r="N24" s="20"/>
-      <c r="O24" s="20"/>
-      <c r="P24" s="20"/>
-      <c r="Q24" s="20"/>
-      <c r="R24" s="20"/>
-      <c r="S24" s="20"/>
-      <c r="T24" s="20"/>
-      <c r="U24" s="20"/>
-      <c r="V24" s="20"/>
-      <c r="W24" s="20"/>
-      <c r="X24" s="20"/>
-      <c r="Y24" s="20"/>
-      <c r="Z24" s="20"/>
-      <c r="AA24" s="20"/>
-      <c r="AB24" s="20"/>
-      <c r="AC24" s="20"/>
-      <c r="AD24" s="20"/>
-      <c r="AE24" s="20"/>
-      <c r="AF24" s="20"/>
-      <c r="AG24" s="20"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="21"/>
+      <c r="K24" s="21"/>
+      <c r="L24" s="21"/>
+      <c r="M24" s="21"/>
+      <c r="N24" s="21"/>
+      <c r="O24" s="21"/>
+      <c r="P24" s="21"/>
+      <c r="Q24" s="21"/>
+      <c r="R24" s="21"/>
+      <c r="S24" s="21"/>
+      <c r="T24" s="21"/>
+      <c r="U24" s="21"/>
+      <c r="V24" s="21"/>
+      <c r="W24" s="21"/>
+      <c r="X24" s="21"/>
+      <c r="Y24" s="21"/>
+      <c r="Z24" s="21"/>
+      <c r="AA24" s="21"/>
+      <c r="AB24" s="21"/>
+      <c r="AC24" s="21"/>
+      <c r="AD24" s="21"/>
+      <c r="AE24" s="21"/>
+      <c r="AF24" s="21"/>
+      <c r="AG24" s="21"/>
       <c r="AH24" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="AI24" s="24" t="n">
+      <c r="AI24" s="25" t="n">
         <v>0.14</v>
       </c>
     </row>
@@ -9856,41 +9856,41 @@
         <f aca="false">Populations!$C$4</f>
         <v>F 15-49</v>
       </c>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="20"/>
-      <c r="I25" s="20"/>
-      <c r="J25" s="20"/>
-      <c r="K25" s="20"/>
-      <c r="L25" s="20"/>
-      <c r="M25" s="20"/>
-      <c r="N25" s="20"/>
-      <c r="O25" s="20"/>
-      <c r="P25" s="20"/>
-      <c r="Q25" s="20"/>
-      <c r="R25" s="20"/>
-      <c r="S25" s="20"/>
-      <c r="T25" s="20"/>
-      <c r="U25" s="20"/>
-      <c r="V25" s="20"/>
-      <c r="W25" s="20"/>
-      <c r="X25" s="20"/>
-      <c r="Y25" s="20"/>
-      <c r="Z25" s="20"/>
-      <c r="AA25" s="20"/>
-      <c r="AB25" s="20"/>
-      <c r="AC25" s="20"/>
-      <c r="AD25" s="20"/>
-      <c r="AE25" s="20"/>
-      <c r="AF25" s="20"/>
-      <c r="AG25" s="20"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="21"/>
+      <c r="K25" s="21"/>
+      <c r="L25" s="21"/>
+      <c r="M25" s="21"/>
+      <c r="N25" s="21"/>
+      <c r="O25" s="21"/>
+      <c r="P25" s="21"/>
+      <c r="Q25" s="21"/>
+      <c r="R25" s="21"/>
+      <c r="S25" s="21"/>
+      <c r="T25" s="21"/>
+      <c r="U25" s="21"/>
+      <c r="V25" s="21"/>
+      <c r="W25" s="21"/>
+      <c r="X25" s="21"/>
+      <c r="Y25" s="21"/>
+      <c r="Z25" s="21"/>
+      <c r="AA25" s="21"/>
+      <c r="AB25" s="21"/>
+      <c r="AC25" s="21"/>
+      <c r="AD25" s="21"/>
+      <c r="AE25" s="21"/>
+      <c r="AF25" s="21"/>
+      <c r="AG25" s="21"/>
       <c r="AH25" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="AI25" s="24" t="n">
+      <c r="AI25" s="25" t="n">
         <v>0.14</v>
       </c>
     </row>
@@ -10002,41 +10002,41 @@
         <f aca="false">Populations!$C$3</f>
         <v>M 15-49</v>
       </c>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="20"/>
-      <c r="I31" s="20"/>
-      <c r="J31" s="20"/>
-      <c r="K31" s="20"/>
-      <c r="L31" s="20"/>
-      <c r="M31" s="20"/>
-      <c r="N31" s="20"/>
-      <c r="O31" s="20"/>
-      <c r="P31" s="20"/>
-      <c r="Q31" s="20"/>
-      <c r="R31" s="20"/>
-      <c r="S31" s="20"/>
-      <c r="T31" s="20"/>
-      <c r="U31" s="20"/>
-      <c r="V31" s="20"/>
-      <c r="W31" s="20"/>
-      <c r="X31" s="20"/>
-      <c r="Y31" s="20"/>
-      <c r="Z31" s="20"/>
-      <c r="AA31" s="20"/>
-      <c r="AB31" s="20"/>
-      <c r="AC31" s="20"/>
-      <c r="AD31" s="20"/>
-      <c r="AE31" s="20"/>
-      <c r="AF31" s="20"/>
-      <c r="AG31" s="20"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="21"/>
+      <c r="H31" s="21"/>
+      <c r="I31" s="21"/>
+      <c r="J31" s="21"/>
+      <c r="K31" s="21"/>
+      <c r="L31" s="21"/>
+      <c r="M31" s="21"/>
+      <c r="N31" s="21"/>
+      <c r="O31" s="21"/>
+      <c r="P31" s="21"/>
+      <c r="Q31" s="21"/>
+      <c r="R31" s="21"/>
+      <c r="S31" s="21"/>
+      <c r="T31" s="21"/>
+      <c r="U31" s="21"/>
+      <c r="V31" s="21"/>
+      <c r="W31" s="21"/>
+      <c r="X31" s="21"/>
+      <c r="Y31" s="21"/>
+      <c r="Z31" s="21"/>
+      <c r="AA31" s="21"/>
+      <c r="AB31" s="21"/>
+      <c r="AC31" s="21"/>
+      <c r="AD31" s="21"/>
+      <c r="AE31" s="21"/>
+      <c r="AF31" s="21"/>
+      <c r="AG31" s="21"/>
       <c r="AH31" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="AI31" s="20" t="n">
+      <c r="AI31" s="21" t="n">
         <v>0.3</v>
       </c>
     </row>
@@ -10045,41 +10045,41 @@
         <f aca="false">Populations!$C$4</f>
         <v>F 15-49</v>
       </c>
-      <c r="C32" s="20"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="20"/>
-      <c r="G32" s="20"/>
-      <c r="H32" s="20"/>
-      <c r="I32" s="20"/>
-      <c r="J32" s="20"/>
-      <c r="K32" s="20"/>
-      <c r="L32" s="20"/>
-      <c r="M32" s="20"/>
-      <c r="N32" s="20"/>
-      <c r="O32" s="20"/>
-      <c r="P32" s="20"/>
-      <c r="Q32" s="20"/>
-      <c r="R32" s="20"/>
-      <c r="S32" s="20"/>
-      <c r="T32" s="20"/>
-      <c r="U32" s="20"/>
-      <c r="V32" s="20"/>
-      <c r="W32" s="20"/>
-      <c r="X32" s="20"/>
-      <c r="Y32" s="20"/>
-      <c r="Z32" s="20"/>
-      <c r="AA32" s="20"/>
-      <c r="AB32" s="20"/>
-      <c r="AC32" s="20"/>
-      <c r="AD32" s="20"/>
-      <c r="AE32" s="20"/>
-      <c r="AF32" s="20"/>
-      <c r="AG32" s="20"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="21"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="21"/>
+      <c r="J32" s="21"/>
+      <c r="K32" s="21"/>
+      <c r="L32" s="21"/>
+      <c r="M32" s="21"/>
+      <c r="N32" s="21"/>
+      <c r="O32" s="21"/>
+      <c r="P32" s="21"/>
+      <c r="Q32" s="21"/>
+      <c r="R32" s="21"/>
+      <c r="S32" s="21"/>
+      <c r="T32" s="21"/>
+      <c r="U32" s="21"/>
+      <c r="V32" s="21"/>
+      <c r="W32" s="21"/>
+      <c r="X32" s="21"/>
+      <c r="Y32" s="21"/>
+      <c r="Z32" s="21"/>
+      <c r="AA32" s="21"/>
+      <c r="AB32" s="21"/>
+      <c r="AC32" s="21"/>
+      <c r="AD32" s="21"/>
+      <c r="AE32" s="21"/>
+      <c r="AF32" s="21"/>
+      <c r="AG32" s="21"/>
       <c r="AH32" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="AI32" s="20" t="n">
+      <c r="AI32" s="21" t="n">
         <v>0.4</v>
       </c>
     </row>
@@ -10191,41 +10191,41 @@
         <f aca="false">Populations!$C$3</f>
         <v>M 15-49</v>
       </c>
-      <c r="C38" s="20"/>
-      <c r="D38" s="20"/>
-      <c r="E38" s="20"/>
-      <c r="F38" s="20"/>
-      <c r="G38" s="20"/>
-      <c r="H38" s="20"/>
-      <c r="I38" s="20"/>
-      <c r="J38" s="20"/>
-      <c r="K38" s="20"/>
-      <c r="L38" s="20"/>
-      <c r="M38" s="20"/>
-      <c r="N38" s="20"/>
-      <c r="O38" s="20"/>
-      <c r="P38" s="20"/>
-      <c r="Q38" s="20"/>
-      <c r="R38" s="20"/>
-      <c r="S38" s="20"/>
-      <c r="T38" s="20"/>
-      <c r="U38" s="20"/>
-      <c r="V38" s="20"/>
-      <c r="W38" s="20"/>
-      <c r="X38" s="20"/>
-      <c r="Y38" s="20"/>
-      <c r="Z38" s="20"/>
-      <c r="AA38" s="20"/>
-      <c r="AB38" s="20"/>
-      <c r="AC38" s="20"/>
-      <c r="AD38" s="20"/>
-      <c r="AE38" s="20"/>
-      <c r="AF38" s="20"/>
-      <c r="AG38" s="20"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="21"/>
+      <c r="H38" s="21"/>
+      <c r="I38" s="21"/>
+      <c r="J38" s="21"/>
+      <c r="K38" s="21"/>
+      <c r="L38" s="21"/>
+      <c r="M38" s="21"/>
+      <c r="N38" s="21"/>
+      <c r="O38" s="21"/>
+      <c r="P38" s="21"/>
+      <c r="Q38" s="21"/>
+      <c r="R38" s="21"/>
+      <c r="S38" s="21"/>
+      <c r="T38" s="21"/>
+      <c r="U38" s="21"/>
+      <c r="V38" s="21"/>
+      <c r="W38" s="21"/>
+      <c r="X38" s="21"/>
+      <c r="Y38" s="21"/>
+      <c r="Z38" s="21"/>
+      <c r="AA38" s="21"/>
+      <c r="AB38" s="21"/>
+      <c r="AC38" s="21"/>
+      <c r="AD38" s="21"/>
+      <c r="AE38" s="21"/>
+      <c r="AF38" s="21"/>
+      <c r="AG38" s="21"/>
       <c r="AH38" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="AI38" s="25" t="n">
+      <c r="AI38" s="26" t="n">
         <v>0</v>
       </c>
     </row>
@@ -10234,41 +10234,41 @@
         <f aca="false">Populations!$C$4</f>
         <v>F 15-49</v>
       </c>
-      <c r="C39" s="20"/>
-      <c r="D39" s="20"/>
-      <c r="E39" s="20"/>
-      <c r="F39" s="20"/>
-      <c r="G39" s="20"/>
-      <c r="H39" s="20"/>
-      <c r="I39" s="20"/>
-      <c r="J39" s="20"/>
-      <c r="K39" s="20"/>
-      <c r="L39" s="20"/>
-      <c r="M39" s="20"/>
-      <c r="N39" s="20"/>
-      <c r="O39" s="20"/>
-      <c r="P39" s="20"/>
-      <c r="Q39" s="20"/>
-      <c r="R39" s="20"/>
-      <c r="S39" s="20"/>
-      <c r="T39" s="20"/>
-      <c r="U39" s="20"/>
-      <c r="V39" s="20"/>
-      <c r="W39" s="20"/>
-      <c r="X39" s="20"/>
-      <c r="Y39" s="20"/>
-      <c r="Z39" s="20"/>
-      <c r="AA39" s="20"/>
-      <c r="AB39" s="20"/>
-      <c r="AC39" s="20"/>
-      <c r="AD39" s="20"/>
-      <c r="AE39" s="20"/>
-      <c r="AF39" s="20"/>
-      <c r="AG39" s="20"/>
+      <c r="C39" s="21"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="21"/>
+      <c r="F39" s="21"/>
+      <c r="G39" s="21"/>
+      <c r="H39" s="21"/>
+      <c r="I39" s="21"/>
+      <c r="J39" s="21"/>
+      <c r="K39" s="21"/>
+      <c r="L39" s="21"/>
+      <c r="M39" s="21"/>
+      <c r="N39" s="21"/>
+      <c r="O39" s="21"/>
+      <c r="P39" s="21"/>
+      <c r="Q39" s="21"/>
+      <c r="R39" s="21"/>
+      <c r="S39" s="21"/>
+      <c r="T39" s="21"/>
+      <c r="U39" s="21"/>
+      <c r="V39" s="21"/>
+      <c r="W39" s="21"/>
+      <c r="X39" s="21"/>
+      <c r="Y39" s="21"/>
+      <c r="Z39" s="21"/>
+      <c r="AA39" s="21"/>
+      <c r="AB39" s="21"/>
+      <c r="AC39" s="21"/>
+      <c r="AD39" s="21"/>
+      <c r="AE39" s="21"/>
+      <c r="AF39" s="21"/>
+      <c r="AG39" s="21"/>
       <c r="AH39" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="AI39" s="24" t="n">
+      <c r="AI39" s="25" t="n">
         <v>0</v>
       </c>
     </row>
@@ -10380,41 +10380,41 @@
         <f aca="false">Populations!$C$3</f>
         <v>M 15-49</v>
       </c>
-      <c r="C45" s="20"/>
-      <c r="D45" s="20"/>
-      <c r="E45" s="20"/>
-      <c r="F45" s="20"/>
-      <c r="G45" s="20"/>
-      <c r="H45" s="20"/>
-      <c r="I45" s="20"/>
-      <c r="J45" s="20"/>
-      <c r="K45" s="20"/>
-      <c r="L45" s="20"/>
-      <c r="M45" s="20"/>
-      <c r="N45" s="20"/>
-      <c r="O45" s="20"/>
-      <c r="P45" s="20"/>
-      <c r="Q45" s="20"/>
-      <c r="R45" s="20"/>
-      <c r="S45" s="20"/>
-      <c r="T45" s="20"/>
-      <c r="U45" s="20"/>
-      <c r="V45" s="20"/>
-      <c r="W45" s="20"/>
-      <c r="X45" s="20"/>
-      <c r="Y45" s="20"/>
-      <c r="Z45" s="20"/>
-      <c r="AA45" s="20"/>
-      <c r="AB45" s="20"/>
-      <c r="AC45" s="20"/>
-      <c r="AD45" s="20"/>
-      <c r="AE45" s="20"/>
-      <c r="AF45" s="20"/>
-      <c r="AG45" s="20"/>
+      <c r="C45" s="21"/>
+      <c r="D45" s="21"/>
+      <c r="E45" s="21"/>
+      <c r="F45" s="21"/>
+      <c r="G45" s="21"/>
+      <c r="H45" s="21"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="21"/>
+      <c r="K45" s="21"/>
+      <c r="L45" s="21"/>
+      <c r="M45" s="21"/>
+      <c r="N45" s="21"/>
+      <c r="O45" s="21"/>
+      <c r="P45" s="21"/>
+      <c r="Q45" s="21"/>
+      <c r="R45" s="21"/>
+      <c r="S45" s="21"/>
+      <c r="T45" s="21"/>
+      <c r="U45" s="21"/>
+      <c r="V45" s="21"/>
+      <c r="W45" s="21"/>
+      <c r="X45" s="21"/>
+      <c r="Y45" s="21"/>
+      <c r="Z45" s="21"/>
+      <c r="AA45" s="21"/>
+      <c r="AB45" s="21"/>
+      <c r="AC45" s="21"/>
+      <c r="AD45" s="21"/>
+      <c r="AE45" s="21"/>
+      <c r="AF45" s="21"/>
+      <c r="AG45" s="21"/>
       <c r="AH45" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="AI45" s="24" t="n">
+      <c r="AI45" s="25" t="n">
         <v>0.1</v>
       </c>
     </row>

</xml_diff>